<commit_message>
Add water data frame, leaks calcs. and leak column to BMP
</commit_message>
<xml_diff>
--- a/experiments/UQ2/gd/UQ2_GD.xlsx
+++ b/experiments/UQ2/gd/UQ2_GD.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup_GD" sheetId="1" r:id="rId1"/>
     <sheet name="Measurements_GD" sheetId="2" r:id="rId2"/>
-    <sheet name="ChangeLog" sheetId="11" r:id="rId3"/>
+    <sheet name="Water" sheetId="14" r:id="rId3"/>
+    <sheet name="ChangeLog" sheetId="11" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -219,10 +220,31 @@
     <t>Inoculum</t>
   </si>
   <si>
-    <t>20.02.2020</t>
-  </si>
-  <si>
     <t>Change filename to UQ2_GD.xlxs</t>
+  </si>
+  <si>
+    <t>Total mass 1 (g)</t>
+  </si>
+  <si>
+    <t>Total mass 2 (g)</t>
+  </si>
+  <si>
+    <t>m.tot1</t>
+  </si>
+  <si>
+    <t>m.tot2</t>
+  </si>
+  <si>
+    <t>27.02.2019</t>
+  </si>
+  <si>
+    <t>20.02.2019</t>
+  </si>
+  <si>
+    <t>UQ2_GD.xlxs</t>
+  </si>
+  <si>
+    <t>Copy water data sheet in from the original UQ2_man_grav.xlsx data</t>
   </si>
 </sst>
 </file>
@@ -234,7 +256,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -287,6 +309,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -349,7 +385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -427,6 +463,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1303,11 +1352,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F93" sqref="F93"/>
+      <selection pane="bottomRight" activeCell="S46" sqref="S46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,10 +4520,679 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>28</v>
+      </c>
+      <c r="B3" s="34">
+        <v>0</v>
+      </c>
+      <c r="C3" s="35">
+        <v>183.8603</v>
+      </c>
+      <c r="D3" s="35">
+        <v>183.86080000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4" s="34">
+        <v>0.84027777777373558</v>
+      </c>
+      <c r="C4" s="35">
+        <v>183.85919999999999</v>
+      </c>
+      <c r="D4" s="35">
+        <v>183.8604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5" s="34">
+        <v>1.84375</v>
+      </c>
+      <c r="C5" s="35">
+        <v>183.8586</v>
+      </c>
+      <c r="D5" s="35">
+        <v>183.86150000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>28</v>
+      </c>
+      <c r="B6" s="34">
+        <v>2.8506944444452529</v>
+      </c>
+      <c r="C6" s="35">
+        <v>183.85759999999999</v>
+      </c>
+      <c r="D6" s="36"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="B7" s="34">
+        <v>3.8090277777737356</v>
+      </c>
+      <c r="C7" s="35">
+        <v>183.8588</v>
+      </c>
+      <c r="D7" s="35">
+        <v>183.85980000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>28</v>
+      </c>
+      <c r="B8" s="34">
+        <v>4.8611111111094942</v>
+      </c>
+      <c r="C8" s="35">
+        <v>183.85720000000001</v>
+      </c>
+      <c r="D8" s="35">
+        <v>183.85669999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="B9" s="34">
+        <v>5.859027777776646</v>
+      </c>
+      <c r="C9" s="35">
+        <v>183.85650000000001</v>
+      </c>
+      <c r="D9" s="35">
+        <v>183.8597</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10" s="34">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="C10" s="35">
+        <v>183.85480000000001</v>
+      </c>
+      <c r="D10" s="35">
+        <v>183.857</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11" s="34">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="C11" s="35">
+        <v>183.85830000000001</v>
+      </c>
+      <c r="D11" s="35">
+        <v>183.85990000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>28</v>
+      </c>
+      <c r="B12" s="34">
+        <v>10.878472222218988</v>
+      </c>
+      <c r="C12" s="35">
+        <v>183.8605</v>
+      </c>
+      <c r="D12" s="35">
+        <v>183.864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>28</v>
+      </c>
+      <c r="B13" s="34">
+        <v>13.125</v>
+      </c>
+      <c r="C13" s="35">
+        <v>183.85929999999999</v>
+      </c>
+      <c r="D13" s="35">
+        <v>183.86089999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14" s="34">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="C14" s="35">
+        <v>183.8587</v>
+      </c>
+      <c r="D14" s="35">
+        <v>183.85910000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>28</v>
+      </c>
+      <c r="B15" s="34">
+        <v>18.909722222218988</v>
+      </c>
+      <c r="C15" s="35">
+        <v>183.85749999999999</v>
+      </c>
+      <c r="D15" s="35">
+        <v>183.8399</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>28</v>
+      </c>
+      <c r="B16" s="34">
+        <v>22.861111111109494</v>
+      </c>
+      <c r="C16" s="35">
+        <v>183.8545</v>
+      </c>
+      <c r="D16" s="35">
+        <v>183.85480000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>28</v>
+      </c>
+      <c r="B17" s="34">
+        <v>27.145833333328483</v>
+      </c>
+      <c r="C17" s="35">
+        <v>183.85329999999999</v>
+      </c>
+      <c r="D17" s="35">
+        <v>183.85310000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>29</v>
+      </c>
+      <c r="B18" s="34">
+        <v>0</v>
+      </c>
+      <c r="C18" s="35">
+        <v>185.58090000000001</v>
+      </c>
+      <c r="D18" s="35">
+        <v>185.58170000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>29</v>
+      </c>
+      <c r="B19" s="34">
+        <v>0.84027777777373558</v>
+      </c>
+      <c r="C19" s="35">
+        <v>185.5797</v>
+      </c>
+      <c r="D19" s="35">
+        <v>185.58189999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>29</v>
+      </c>
+      <c r="B20" s="34">
+        <v>1.84375</v>
+      </c>
+      <c r="C20" s="35">
+        <v>185.57980000000001</v>
+      </c>
+      <c r="D20" s="35">
+        <v>185.583</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>29</v>
+      </c>
+      <c r="B21" s="34">
+        <v>2.8506944444452529</v>
+      </c>
+      <c r="C21" s="35">
+        <v>185.5787</v>
+      </c>
+      <c r="D21" s="36"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>29</v>
+      </c>
+      <c r="B22" s="34">
+        <v>3.8090277777737356</v>
+      </c>
+      <c r="C22" s="35">
+        <v>185.58080000000001</v>
+      </c>
+      <c r="D22" s="35">
+        <v>185.58019999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>29</v>
+      </c>
+      <c r="B23" s="34">
+        <v>4.8611111111094942</v>
+      </c>
+      <c r="C23" s="35">
+        <v>185.5788</v>
+      </c>
+      <c r="D23" s="35">
+        <v>185.57929999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24" s="34">
+        <v>5.859027777776646</v>
+      </c>
+      <c r="C24" s="35">
+        <v>185.5804</v>
+      </c>
+      <c r="D24" s="35">
+        <v>185.58170000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>29</v>
+      </c>
+      <c r="B25" s="34">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="C25" s="35">
+        <v>185.57849999999999</v>
+      </c>
+      <c r="D25" s="35">
+        <v>185.57859999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26" s="34">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="C26" s="35">
+        <v>185.58179999999999</v>
+      </c>
+      <c r="D26" s="35">
+        <v>185.5831</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>29</v>
+      </c>
+      <c r="B27" s="34">
+        <v>10.878472222218988</v>
+      </c>
+      <c r="C27" s="35">
+        <v>185.58420000000001</v>
+      </c>
+      <c r="D27" s="35">
+        <v>185.58779999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>29</v>
+      </c>
+      <c r="B28" s="34">
+        <v>13.125</v>
+      </c>
+      <c r="C28" s="35">
+        <v>185.5847</v>
+      </c>
+      <c r="D28" s="35">
+        <v>185.5857</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+      <c r="B29" s="34">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="C29" s="35">
+        <v>185.58369999999999</v>
+      </c>
+      <c r="D29" s="35">
+        <v>185.58410000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="34">
+        <v>18.909722222218988</v>
+      </c>
+      <c r="C30" s="35">
+        <v>185.58260000000001</v>
+      </c>
+      <c r="D30" s="35">
+        <v>185.5857</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" s="34">
+        <v>22.861111111109494</v>
+      </c>
+      <c r="C31" s="35">
+        <v>185.5787</v>
+      </c>
+      <c r="D31" s="35">
+        <v>185.57990000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="34">
+        <v>27.145833333328483</v>
+      </c>
+      <c r="C32" s="35">
+        <v>185.5788</v>
+      </c>
+      <c r="D32" s="35">
+        <v>185.57900000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="34">
+        <v>0</v>
+      </c>
+      <c r="C33" s="35">
+        <v>183.7165</v>
+      </c>
+      <c r="D33" s="35">
+        <v>183.7176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34" s="34">
+        <v>0.84027777777373558</v>
+      </c>
+      <c r="C34" s="35">
+        <v>183.71619999999999</v>
+      </c>
+      <c r="D34" s="35">
+        <v>183.71799999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35" s="34">
+        <v>1.84375</v>
+      </c>
+      <c r="C35" s="35">
+        <v>183.71600000000001</v>
+      </c>
+      <c r="D35" s="35">
+        <v>183.7182</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36" s="34">
+        <v>2.8506944444452529</v>
+      </c>
+      <c r="C36" s="35">
+        <v>183.7148</v>
+      </c>
+      <c r="D36" s="36"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" s="34">
+        <v>3.8090277777737356</v>
+      </c>
+      <c r="C37" s="35">
+        <v>183.71600000000001</v>
+      </c>
+      <c r="D37" s="37">
+        <v>183.71629999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>30</v>
+      </c>
+      <c r="B38" s="34">
+        <v>4.8611111111094942</v>
+      </c>
+      <c r="C38" s="35">
+        <v>183.715</v>
+      </c>
+      <c r="D38" s="35">
+        <v>183.7157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>30</v>
+      </c>
+      <c r="B39" s="34">
+        <v>5.859027777776646</v>
+      </c>
+      <c r="C39" s="35">
+        <v>183.7157</v>
+      </c>
+      <c r="D39" s="35">
+        <v>183.71809999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>30</v>
+      </c>
+      <c r="B40" s="34">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="C40" s="35">
+        <v>183.71369999999999</v>
+      </c>
+      <c r="D40" s="35">
+        <v>183.71420000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41" s="34">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="C41" s="35">
+        <v>183.7174</v>
+      </c>
+      <c r="D41" s="35">
+        <v>183.71780000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>30</v>
+      </c>
+      <c r="B42" s="34">
+        <v>10.878472222218988</v>
+      </c>
+      <c r="C42" s="35">
+        <v>183.7199</v>
+      </c>
+      <c r="D42" s="35">
+        <v>183.72280000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43" s="34">
+        <v>13.125</v>
+      </c>
+      <c r="C43" s="35">
+        <v>183.72040000000001</v>
+      </c>
+      <c r="D43" s="35">
+        <v>183.72110000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>30</v>
+      </c>
+      <c r="B44" s="34">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="C44" s="35">
+        <v>183.71850000000001</v>
+      </c>
+      <c r="D44" s="35">
+        <v>183.71899999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>30</v>
+      </c>
+      <c r="B45" s="34">
+        <v>18.909722222218988</v>
+      </c>
+      <c r="C45" s="35">
+        <v>183.71690000000001</v>
+      </c>
+      <c r="D45" s="35">
+        <v>183.72110000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>30</v>
+      </c>
+      <c r="B46" s="34">
+        <v>22.861111111109494</v>
+      </c>
+      <c r="C46" s="35">
+        <v>183.71279999999999</v>
+      </c>
+      <c r="D46" s="35">
+        <v>183.71469999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>30</v>
+      </c>
+      <c r="B47" s="34">
+        <v>27.145833333328483</v>
+      </c>
+      <c r="C47" s="35">
+        <v>183.71299999999999</v>
+      </c>
+      <c r="D47" s="35">
+        <v>183.71420000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4529,7 +5247,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>51</v>
@@ -4538,7 +5256,21 @@
         <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add diferent methods for cumBgGD function and xCH4 plots + mad some changes in excel file
</commit_message>
<xml_diff>
--- a/experiments/UQ2/gd/UQ2_GD.xlsx
+++ b/experiments/UQ2/gd/UQ2_GD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Setup_GD" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="74">
   <si>
     <t>id</t>
   </si>
@@ -245,6 +245,15 @@
   </si>
   <si>
     <t>Copy water data sheet in from the original UQ2_man_grav.xlsx data</t>
+  </si>
+  <si>
+    <t>28.02.2019</t>
+  </si>
+  <si>
+    <t>Add 0 in volume for day 0</t>
+  </si>
+  <si>
+    <t>Add mas.init = mass.final instead of having empty rows to avoid NA problem in R</t>
   </si>
 </sst>
 </file>
@@ -1353,10 +1362,10 @@
   <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S46" sqref="S46"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,193 +1447,207 @@
       <c r="D3" s="12">
         <v>1230</v>
       </c>
-      <c r="E3"/>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="32">
+        <f>G3</f>
+        <v>183.26605000000001</v>
+      </c>
       <c r="G3" s="32">
         <v>183.26605000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="12">
-        <v>13112018</v>
+        <v>12112018</v>
       </c>
       <c r="C4" s="24">
-        <v>0.84027777777373558</v>
+        <v>0</v>
       </c>
       <c r="D4" s="12">
-        <v>840</v>
+        <v>1230</v>
       </c>
       <c r="E4" s="12">
-        <v>27</v>
-      </c>
-      <c r="F4" s="26">
-        <v>183.26509999999999</v>
+        <v>0</v>
+      </c>
+      <c r="F4" s="32">
+        <f t="shared" ref="F4:F11" si="0">G4</f>
+        <v>183.88749999999999</v>
       </c>
       <c r="G4" s="32">
-        <v>183.23079999999999</v>
+        <v>183.88749999999999</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B5" s="12">
-        <v>14112018</v>
+        <v>12112018</v>
       </c>
       <c r="C5" s="24">
-        <v>1.84375</v>
+        <v>0</v>
       </c>
       <c r="D5" s="12">
-        <v>845</v>
+        <v>1230</v>
       </c>
       <c r="E5" s="12">
-        <v>17.5</v>
-      </c>
-      <c r="F5" s="26">
-        <v>183.23249999999999</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="32">
+        <f t="shared" si="0"/>
+        <v>183.7484</v>
       </c>
       <c r="G5" s="32">
-        <v>183.21039999999999</v>
+        <v>183.7484</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B6" s="12">
-        <v>15112018</v>
+        <v>12112018</v>
       </c>
       <c r="C6" s="24">
-        <v>2.8506944444452529</v>
+        <v>0</v>
       </c>
       <c r="D6" s="12">
-        <v>855</v>
+        <v>1230</v>
       </c>
       <c r="E6" s="12">
-        <v>14</v>
-      </c>
-      <c r="F6" s="26">
-        <v>183.20679999999999</v>
+        <v>0</v>
+      </c>
+      <c r="F6" s="32">
+        <f t="shared" si="0"/>
+        <v>185.28739999999999</v>
       </c>
       <c r="G6" s="32">
-        <v>183.19</v>
+        <v>185.28739999999999</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B7" s="12">
-        <v>16112018</v>
+        <v>12112018</v>
       </c>
       <c r="C7" s="24">
-        <v>3.8090277777737356</v>
+        <v>0</v>
       </c>
       <c r="D7" s="12">
-        <v>755</v>
+        <v>1230</v>
       </c>
       <c r="E7" s="12">
-        <v>11</v>
-      </c>
-      <c r="F7" s="26">
-        <v>183.19130000000001</v>
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <f t="shared" si="0"/>
+        <v>188.50425000000001</v>
       </c>
       <c r="G7" s="32">
-        <v>183.17789999999999</v>
+        <v>188.50425000000001</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B8" s="12">
-        <v>17112018</v>
+        <v>12112018</v>
       </c>
       <c r="C8" s="24">
-        <v>4.8611111111094942</v>
+        <v>0</v>
       </c>
       <c r="D8" s="12">
-        <v>910</v>
+        <v>1230</v>
       </c>
       <c r="E8" s="12">
-        <v>8.5</v>
-      </c>
-      <c r="F8" s="26">
-        <v>183.17750000000001</v>
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
+        <f t="shared" si="0"/>
+        <v>184.17580000000001</v>
       </c>
       <c r="G8" s="32">
-        <v>183.16659999999999</v>
+        <v>184.17580000000001</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="B9" s="12">
-        <v>18112018</v>
+        <v>12112018</v>
       </c>
       <c r="C9" s="24">
-        <v>5.859027777776646</v>
+        <v>0</v>
       </c>
       <c r="D9" s="12">
-        <v>907</v>
+        <v>1230</v>
       </c>
       <c r="E9" s="12">
-        <v>7.8</v>
-      </c>
-      <c r="F9" s="26">
-        <v>183.16909999999999</v>
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <f t="shared" si="0"/>
+        <v>188.87815000000001</v>
       </c>
       <c r="G9" s="32">
-        <v>183.16</v>
+        <v>188.87815000000001</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B10" s="12">
-        <v>19112018</v>
+        <v>12112018</v>
       </c>
       <c r="C10" s="24">
-        <v>6.8395833333343035</v>
+        <v>0</v>
       </c>
       <c r="D10" s="12">
-        <v>839</v>
+        <v>1230</v>
       </c>
       <c r="E10" s="12">
-        <v>7.5</v>
-      </c>
-      <c r="F10" s="26">
-        <v>183.15600000000001</v>
+        <v>0</v>
+      </c>
+      <c r="F10" s="32">
+        <f t="shared" si="0"/>
+        <v>185.49180000000001</v>
       </c>
       <c r="G10" s="32">
-        <v>183.1473</v>
+        <v>185.49180000000001</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="B11" s="12">
-        <v>21112018</v>
+        <v>12112018</v>
       </c>
       <c r="C11" s="24">
-        <v>8.9166666666642413</v>
+        <v>0</v>
       </c>
       <c r="D11" s="12">
-        <v>1030</v>
+        <v>1230</v>
       </c>
       <c r="E11" s="12">
-        <v>12.8</v>
-      </c>
-      <c r="F11" s="26">
-        <v>183.1523</v>
+        <v>0</v>
+      </c>
+      <c r="F11" s="32">
+        <f t="shared" si="0"/>
+        <v>184.33615</v>
       </c>
       <c r="G11" s="32">
-        <v>183.13749999999999</v>
+        <v>184.33615</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1632,160 +1655,166 @@
         <v>57</v>
       </c>
       <c r="B12" s="12">
-        <v>23112018</v>
+        <v>13112018</v>
       </c>
       <c r="C12" s="24">
-        <v>10.878472222218988</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D12" s="12">
-        <v>935</v>
+        <v>840</v>
       </c>
       <c r="E12" s="12">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F12" s="26">
-        <v>183.1396</v>
+        <v>183.26509999999999</v>
       </c>
       <c r="G12" s="32">
-        <v>183.1276</v>
+        <v>183.23079999999999</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B13" s="12">
-        <v>25112018</v>
+        <v>13112018</v>
       </c>
       <c r="C13" s="24">
-        <v>13.125</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D13" s="12">
-        <v>1530</v>
+        <v>840</v>
       </c>
       <c r="E13" s="12">
-        <v>12.66</v>
+        <v>28</v>
       </c>
       <c r="F13" s="26">
-        <v>183.12700000000001</v>
+        <v>183.88720000000001</v>
       </c>
       <c r="G13" s="32">
-        <v>183.11240000000001</v>
+        <v>183.851</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B14" s="12">
-        <v>28112018</v>
+        <v>13112018</v>
       </c>
       <c r="C14" s="24">
-        <v>15.854166666664241</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D14" s="12">
-        <v>900</v>
+        <v>840</v>
       </c>
       <c r="E14" s="12">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="F14" s="26">
-        <v>183.11019999999999</v>
+        <v>183.74780000000001</v>
       </c>
       <c r="G14" s="32">
-        <v>183.09610000000001</v>
+        <v>183.7115</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B15" s="12">
-        <v>1122018</v>
+        <v>13112018</v>
       </c>
       <c r="C15" s="24">
-        <v>18.909722222218988</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D15" s="12">
-        <v>1020</v>
+        <v>840</v>
       </c>
       <c r="E15" s="12">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F15" s="26">
-        <v>183.09690000000001</v>
+        <v>185.28700000000001</v>
       </c>
       <c r="G15" s="32">
-        <v>183.08510000000001</v>
+        <v>185.24809999999999</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B16" s="12">
-        <v>5122018</v>
+        <v>13112018</v>
       </c>
       <c r="C16" s="24">
-        <v>22.861111111109494</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D16" s="12">
-        <v>910</v>
+        <v>840</v>
       </c>
       <c r="E16" s="12">
-        <v>11.1</v>
+        <v>31</v>
       </c>
       <c r="F16" s="26">
-        <v>183.0789</v>
+        <v>188.5035</v>
       </c>
       <c r="G16" s="32">
-        <v>183.06549999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188.4641</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B17" s="12">
-        <v>9122018</v>
+        <v>13112018</v>
       </c>
       <c r="C17" s="24">
-        <v>27.145833333328483</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D17" s="12">
-        <v>1600</v>
+        <v>840</v>
       </c>
       <c r="E17" s="12">
-        <v>13</v>
+        <v>28.5</v>
       </c>
       <c r="F17" s="26">
-        <v>183.06450000000001</v>
+        <v>184.1746</v>
       </c>
       <c r="G17" s="32">
-        <v>183.04900000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>184.13939999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B18" s="12">
-        <v>12112018</v>
+        <v>13112018</v>
       </c>
       <c r="C18" s="24">
-        <v>0</v>
+        <v>0.84027777777373558</v>
       </c>
       <c r="D18" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E18"/>
+        <v>840</v>
+      </c>
+      <c r="E18" s="12">
+        <f>50+50+38</f>
+        <v>138</v>
+      </c>
+      <c r="F18" s="26">
+        <v>188.87790000000001</v>
+      </c>
       <c r="G18" s="32">
-        <v>183.88749999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188.71129999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="B19" s="12">
         <v>13112018</v>
@@ -1797,383 +1826,392 @@
         <v>840</v>
       </c>
       <c r="E19" s="12">
-        <v>28</v>
+        <v>135.5</v>
       </c>
       <c r="F19" s="26">
-        <v>183.88720000000001</v>
+        <v>185.49119999999999</v>
       </c>
       <c r="G19" s="32">
-        <v>183.851</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185.3244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B20" s="12">
+        <v>13112018</v>
+      </c>
+      <c r="C20" s="24">
+        <v>0.84027777777373558</v>
+      </c>
+      <c r="D20" s="12">
+        <v>840</v>
+      </c>
+      <c r="E20" s="12">
+        <v>140.5</v>
+      </c>
+      <c r="F20" s="26">
+        <v>184.33600000000001</v>
+      </c>
+      <c r="G20" s="32">
+        <v>184.16579999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" s="12">
         <v>14112018</v>
       </c>
-      <c r="C20" s="24">
+      <c r="C21" s="24">
         <v>1.84375</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D21" s="12">
         <v>845</v>
       </c>
-      <c r="E20" s="12">
-        <v>18.25</v>
-      </c>
-      <c r="F20" s="26">
-        <v>183.85230000000001</v>
-      </c>
-      <c r="G20" s="32">
-        <v>183.82910000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="12">
-        <v>15112018</v>
-      </c>
-      <c r="C21" s="24">
-        <v>2.8506944444452529</v>
-      </c>
-      <c r="D21" s="12">
-        <v>855</v>
-      </c>
       <c r="E21" s="12">
-        <v>14.25</v>
+        <v>17.5</v>
       </c>
       <c r="F21" s="26">
-        <v>183.8263</v>
+        <v>183.23249999999999</v>
       </c>
       <c r="G21" s="32">
-        <v>183.80850000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183.21039999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="12">
-        <v>16112018</v>
+        <v>14112018</v>
       </c>
       <c r="C22" s="24">
-        <v>3.8090277777737356</v>
+        <v>1.84375</v>
       </c>
       <c r="D22" s="12">
-        <v>755</v>
+        <v>845</v>
       </c>
       <c r="E22" s="12">
-        <v>13</v>
+        <v>18.25</v>
       </c>
       <c r="F22" s="26">
-        <v>183.81059999999999</v>
+        <v>183.85230000000001</v>
       </c>
       <c r="G22" s="32">
-        <v>183.79470000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183.82910000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B23" s="12">
-        <v>17112018</v>
+        <v>14112018</v>
       </c>
       <c r="C23" s="24">
-        <v>4.8611111111094942</v>
+        <v>1.84375</v>
       </c>
       <c r="D23" s="12">
-        <v>910</v>
+        <v>845</v>
       </c>
       <c r="E23" s="12">
-        <v>9.9</v>
+        <v>18.25</v>
       </c>
       <c r="F23" s="26">
-        <v>183.7938</v>
+        <v>183.71250000000001</v>
       </c>
       <c r="G23" s="32">
-        <v>183.78229999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183.69030000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B24" s="12">
-        <v>18112018</v>
+        <v>14112018</v>
       </c>
       <c r="C24" s="24">
-        <v>5.859027777776646</v>
+        <v>1.84375</v>
       </c>
       <c r="D24" s="12">
-        <v>907</v>
+        <v>845</v>
       </c>
       <c r="E24" s="12">
-        <v>9.1999999999999993</v>
+        <v>48.5</v>
       </c>
       <c r="F24" s="26">
-        <v>183.78399999999999</v>
+        <v>185.2492</v>
       </c>
       <c r="G24" s="32">
-        <v>183.7731</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185.19730000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="B25" s="12">
-        <v>19112018</v>
+        <v>14112018</v>
       </c>
       <c r="C25" s="24">
-        <v>6.8395833333343035</v>
+        <v>1.84375</v>
       </c>
       <c r="D25" s="12">
-        <v>839</v>
+        <v>845</v>
       </c>
       <c r="E25" s="12">
-        <v>8.1</v>
+        <v>48</v>
       </c>
       <c r="F25" s="26">
-        <v>183.77019999999999</v>
+        <v>188.46549999999999</v>
       </c>
       <c r="G25" s="32">
-        <v>183.7604</v>
-      </c>
-      <c r="H25" s="25"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188.4084</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="B26" s="12">
-        <v>21112018</v>
+        <v>14112018</v>
       </c>
       <c r="C26" s="24">
-        <v>8.9166666666642413</v>
+        <v>1.84375</v>
       </c>
       <c r="D26" s="12">
-        <v>1030</v>
+        <v>845</v>
       </c>
       <c r="E26" s="12">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F26" s="26">
-        <v>183.76429999999999</v>
+        <v>184.1405</v>
       </c>
       <c r="G26" s="32">
-        <v>183.74770000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>184.08320000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="B27" s="12">
-        <v>23112018</v>
+        <v>14112018</v>
       </c>
       <c r="C27" s="24">
-        <v>10.878472222218988</v>
+        <v>1.84375</v>
       </c>
       <c r="D27" s="12">
-        <v>935</v>
+        <v>845</v>
       </c>
       <c r="E27" s="12">
-        <v>10.75</v>
+        <f>53+37+31.6+51.3</f>
+        <v>172.89999999999998</v>
       </c>
       <c r="F27" s="26">
-        <v>183.75149999999999</v>
+        <v>188.71180000000001</v>
       </c>
       <c r="G27" s="32">
-        <v>183.73779999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>188.5119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>58</v>
+        <v>9</v>
       </c>
       <c r="B28" s="12">
-        <v>25112018</v>
+        <v>14112018</v>
       </c>
       <c r="C28" s="24">
-        <v>13.125</v>
+        <v>1.84375</v>
       </c>
       <c r="D28" s="12">
-        <v>1530</v>
+        <v>845</v>
       </c>
       <c r="E28" s="12">
-        <v>13.33</v>
-      </c>
-      <c r="F28" s="30">
-        <v>183.73650000000001</v>
+        <f>30+56.3+44+44</f>
+        <v>174.3</v>
+      </c>
+      <c r="F28" s="26">
+        <v>185.3254</v>
       </c>
       <c r="G28" s="32">
-        <v>183.7217</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>185.12260000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="B29" s="12">
-        <v>28112018</v>
+        <v>14112018</v>
       </c>
       <c r="C29" s="24">
-        <v>15.854166666664241</v>
+        <v>1.84375</v>
       </c>
       <c r="D29" s="12">
-        <v>900</v>
+        <v>845</v>
       </c>
       <c r="E29" s="12">
-        <v>13</v>
+        <f>35.2+54.5+40.5+43.8</f>
+        <v>174</v>
       </c>
       <c r="F29" s="26">
-        <v>183.721</v>
+        <v>184.16659999999999</v>
       </c>
       <c r="G29" s="32">
-        <v>183.70490000000001</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183.96469999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="12">
-        <v>1122018</v>
+        <v>15112018</v>
       </c>
       <c r="C30" s="24">
-        <v>18.909722222218988</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D30" s="12">
-        <v>1020</v>
+        <v>855</v>
       </c>
       <c r="E30" s="12">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F30" s="26">
-        <v>183.70509999999999</v>
+        <v>183.20679999999999</v>
       </c>
       <c r="G30" s="32">
-        <v>183.69239999999999</v>
-      </c>
-      <c r="H30" s="25"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183.19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="12">
-        <v>5122018</v>
+        <v>15112018</v>
       </c>
       <c r="C31" s="24">
-        <v>22.861111111109494</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D31" s="12">
-        <v>910</v>
+        <v>855</v>
       </c>
       <c r="E31" s="12">
-        <v>12</v>
+        <v>14.25</v>
       </c>
       <c r="F31" s="26">
-        <v>183.6875</v>
+        <v>183.8263</v>
       </c>
       <c r="G31" s="32">
-        <v>183.67359999999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>183.80850000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" s="12">
-        <v>9122018</v>
+        <v>15112018</v>
       </c>
       <c r="C32" s="24">
-        <v>27.145833333328483</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D32" s="12">
-        <v>1600</v>
+        <v>855</v>
       </c>
       <c r="E32" s="12">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F32" s="26">
-        <v>183.67250000000001</v>
+        <v>183.68729999999999</v>
       </c>
       <c r="G32" s="32">
-        <v>183.65950000000001</v>
+        <v>183.66839999999999</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B33" s="12">
-        <v>12112018</v>
+        <v>15112018</v>
       </c>
       <c r="C33" s="24">
-        <v>0</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D33" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E33"/>
+        <v>855</v>
+      </c>
+      <c r="E33" s="12">
+        <f>24+51+24+57</f>
+        <v>156</v>
+      </c>
+      <c r="F33" s="26">
+        <v>185.19399999999999</v>
+      </c>
       <c r="G33" s="32">
-        <v>183.7484</v>
+        <v>185.0059</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B34" s="12">
-        <v>13112018</v>
+        <v>15112018</v>
       </c>
       <c r="C34" s="24">
-        <v>0.84027777777373558</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D34" s="12">
-        <v>840</v>
+        <v>855</v>
       </c>
       <c r="E34" s="12">
-        <v>28</v>
+        <f>57+29.6+44.5+36.6</f>
+        <v>167.7</v>
       </c>
       <c r="F34" s="26">
-        <v>183.74780000000001</v>
+        <v>188.4049</v>
       </c>
       <c r="G34" s="32">
-        <v>183.7115</v>
+        <v>188.2022</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B35" s="12">
-        <v>14112018</v>
+        <v>15112018</v>
       </c>
       <c r="C35" s="24">
-        <v>1.84375</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D35" s="12">
-        <v>845</v>
+        <v>855</v>
       </c>
       <c r="E35" s="12">
-        <v>18.25</v>
+        <f>35+51.6+37+40</f>
+        <v>163.6</v>
       </c>
       <c r="F35" s="26">
-        <v>183.71250000000001</v>
+        <v>184.0796</v>
       </c>
       <c r="G35" s="32">
-        <v>183.69030000000001</v>
+        <v>183.88130000000001</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B36" s="12">
         <v>15112018</v>
@@ -2185,105 +2223,108 @@
         <v>855</v>
       </c>
       <c r="E36" s="12">
-        <v>15</v>
+        <f>35.5+45.25+35.25+49.5</f>
+        <v>165.5</v>
       </c>
       <c r="F36" s="26">
-        <v>183.68729999999999</v>
+        <v>188.50700000000001</v>
       </c>
       <c r="G36" s="32">
-        <v>183.66839999999999</v>
+        <v>188.328</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B37" s="12">
-        <v>16112018</v>
+        <v>15112018</v>
       </c>
       <c r="C37" s="24">
-        <v>3.8090277777737356</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D37" s="12">
-        <v>755</v>
+        <v>855</v>
       </c>
       <c r="E37" s="12">
-        <v>11.5</v>
+        <f>48.5+37.5+40+42</f>
+        <v>168</v>
       </c>
       <c r="F37" s="26">
-        <v>183.6695</v>
+        <v>185.11920000000001</v>
       </c>
       <c r="G37" s="32">
-        <v>183.65479999999999</v>
+        <v>184.93819999999999</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="B38" s="12">
-        <v>17112018</v>
+        <v>15112018</v>
       </c>
       <c r="C38" s="24">
-        <v>4.8611111111094942</v>
+        <v>2.8506944444452529</v>
       </c>
       <c r="D38" s="12">
-        <v>910</v>
+        <v>855</v>
       </c>
       <c r="E38" s="12">
-        <v>10.8</v>
+        <f>41+25.5+58+42</f>
+        <v>166.5</v>
       </c>
       <c r="F38" s="26">
-        <v>183.65289999999999</v>
+        <v>183.96039999999999</v>
       </c>
       <c r="G38" s="32">
-        <v>183.6405</v>
+        <v>183.7807</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B39" s="12">
-        <v>18112018</v>
+        <v>16112018</v>
       </c>
       <c r="C39" s="24">
-        <v>5.859027777776646</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D39" s="12">
-        <v>907</v>
+        <v>755</v>
       </c>
       <c r="E39" s="12">
-        <v>8.1999999999999993</v>
+        <v>11</v>
       </c>
       <c r="F39" s="26">
-        <v>183.64330000000001</v>
+        <v>183.19130000000001</v>
       </c>
       <c r="G39" s="32">
-        <v>183.63380000000001</v>
+        <v>183.17789999999999</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="12">
-        <v>19112018</v>
+        <v>16112018</v>
       </c>
       <c r="C40" s="24">
-        <v>6.8395833333343035</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D40" s="12">
-        <v>839</v>
+        <v>755</v>
       </c>
       <c r="E40" s="12">
-        <v>7.2</v>
+        <v>13</v>
       </c>
       <c r="F40" s="26">
-        <v>183.63130000000001</v>
+        <v>183.81059999999999</v>
       </c>
       <c r="G40" s="32">
-        <v>183.62280000000001</v>
+        <v>183.79470000000001</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2291,224 +2332,235 @@
         <v>59</v>
       </c>
       <c r="B41" s="12">
-        <v>21112018</v>
+        <v>16112018</v>
       </c>
       <c r="C41" s="24">
-        <v>8.9166666666642413</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D41" s="12">
-        <v>1030</v>
+        <v>755</v>
       </c>
       <c r="E41" s="12">
-        <v>13.1</v>
+        <v>11.5</v>
       </c>
       <c r="F41" s="26">
-        <v>183.62649999999999</v>
+        <v>183.6695</v>
       </c>
       <c r="G41" s="32">
-        <v>183.61080000000001</v>
+        <v>183.65479999999999</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="B42" s="12">
-        <v>23112018</v>
+        <v>16112018</v>
       </c>
       <c r="C42" s="24">
-        <v>10.878472222218988</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D42" s="12">
-        <v>935</v>
+        <v>755</v>
       </c>
       <c r="E42" s="12">
-        <v>11</v>
+        <f>43+49+44+50</f>
+        <v>186</v>
       </c>
       <c r="F42" s="26">
-        <v>183.61439999999999</v>
+        <v>185.00630000000001</v>
       </c>
       <c r="G42" s="32">
-        <v>183.6018</v>
+        <v>184.7724</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B43" s="12">
-        <v>25112018</v>
+        <v>16112018</v>
       </c>
       <c r="C43" s="24">
-        <v>13.125</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D43" s="12">
-        <v>1530</v>
+        <v>755</v>
       </c>
       <c r="E43" s="12">
-        <v>12.33</v>
+        <f>38+52+42+50</f>
+        <v>182</v>
       </c>
       <c r="F43" s="26">
-        <v>183.6009</v>
+        <v>188.20359999999999</v>
       </c>
       <c r="G43" s="32">
-        <v>183.58670000000001</v>
+        <v>187.97470000000001</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B44" s="12">
-        <v>28112018</v>
+        <v>16112018</v>
       </c>
       <c r="C44" s="24">
-        <v>15.854166666664241</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D44" s="12">
-        <v>900</v>
+        <v>755</v>
       </c>
       <c r="E44" s="12">
-        <v>12.33</v>
+        <f>41+47.5+50+40.25</f>
+        <v>178.75</v>
       </c>
       <c r="F44" s="26">
-        <v>183.5848</v>
+        <v>183.88200000000001</v>
       </c>
       <c r="G44" s="32">
-        <v>183.57140000000001</v>
+        <v>183.6568</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="B45" s="12">
-        <v>1122018</v>
+        <v>16112018</v>
       </c>
       <c r="C45" s="24">
-        <v>18.909722222218988</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D45" s="12">
-        <v>1020</v>
+        <v>755</v>
       </c>
       <c r="E45" s="12">
-        <v>11</v>
+        <f>29.66+21+22+28.5</f>
+        <v>101.16</v>
       </c>
       <c r="F45" s="26">
-        <v>183.5727</v>
+        <v>188.3279</v>
       </c>
       <c r="G45" s="32">
-        <v>183.5592</v>
+        <v>188.22149999999999</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="B46" s="12">
-        <v>5122018</v>
+        <v>16112018</v>
       </c>
       <c r="C46" s="24">
-        <v>22.861111111109494</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D46" s="12">
-        <v>910</v>
+        <v>755</v>
       </c>
       <c r="E46" s="12">
-        <v>11.8</v>
+        <f>53+45</f>
+        <v>98</v>
       </c>
       <c r="F46" s="26">
-        <v>183.55459999999999</v>
+        <v>184.9402</v>
       </c>
       <c r="G46" s="32">
-        <v>183.53960000000001</v>
+        <v>184.833</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="B47" s="12">
-        <v>9122018</v>
+        <v>16112018</v>
       </c>
       <c r="C47" s="24">
-        <v>27.145833333328483</v>
+        <v>3.8090277777737356</v>
       </c>
       <c r="D47" s="12">
-        <v>1600</v>
+        <v>755</v>
       </c>
       <c r="E47" s="12">
-        <v>11.6</v>
+        <f>50.25+49.5</f>
+        <v>99.75</v>
       </c>
       <c r="F47" s="26">
-        <v>183.53899999999999</v>
+        <v>183.78370000000001</v>
       </c>
       <c r="G47" s="32">
-        <v>183.52619999999999</v>
+        <v>183.67580000000001</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B48" s="12">
-        <v>12112018</v>
+        <v>17112018</v>
       </c>
       <c r="C48" s="24">
-        <v>0</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D48" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E48"/>
+        <v>910</v>
+      </c>
+      <c r="E48" s="12">
+        <v>8.5</v>
+      </c>
+      <c r="F48" s="26">
+        <v>183.17750000000001</v>
+      </c>
       <c r="G48" s="32">
-        <v>185.28739999999999</v>
+        <v>183.16659999999999</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B49" s="12">
-        <v>13112018</v>
+        <v>17112018</v>
       </c>
       <c r="C49" s="24">
-        <v>0.84027777777373558</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D49" s="12">
-        <v>840</v>
+        <v>910</v>
       </c>
       <c r="E49" s="12">
-        <v>30</v>
+        <v>9.9</v>
       </c>
       <c r="F49" s="26">
-        <v>185.28700000000001</v>
+        <v>183.7938</v>
       </c>
       <c r="G49" s="32">
-        <v>185.24809999999999</v>
+        <v>183.78229999999999</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B50" s="12">
-        <v>14112018</v>
+        <v>17112018</v>
       </c>
       <c r="C50" s="24">
-        <v>1.84375</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D50" s="12">
-        <v>845</v>
+        <v>910</v>
       </c>
       <c r="E50" s="12">
-        <v>48.5</v>
+        <v>10.8</v>
       </c>
       <c r="F50" s="26">
-        <v>185.2492</v>
+        <v>183.65289999999999</v>
       </c>
       <c r="G50" s="32">
-        <v>185.19730000000001</v>
+        <v>183.6405</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2516,52 +2568,52 @@
         <v>40</v>
       </c>
       <c r="B51" s="12">
-        <v>15112018</v>
+        <v>17112018</v>
       </c>
       <c r="C51" s="24">
-        <v>2.8506944444452529</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D51" s="12">
-        <v>855</v>
+        <v>910</v>
       </c>
       <c r="E51" s="12">
-        <f>24+51+24+57</f>
-        <v>156</v>
+        <f>45.5+58+25</f>
+        <v>128.5</v>
       </c>
       <c r="F51" s="26">
-        <v>185.19399999999999</v>
+        <v>184.77180000000001</v>
       </c>
       <c r="G51" s="32">
-        <v>185.0059</v>
+        <v>184.60230000000001</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B52" s="12">
-        <v>16112018</v>
+        <v>17112018</v>
       </c>
       <c r="C52" s="24">
-        <v>3.8090277777737356</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D52" s="12">
-        <v>755</v>
+        <v>910</v>
       </c>
       <c r="E52" s="12">
-        <f>43+49+44+50</f>
-        <v>186</v>
+        <f>48+23+53</f>
+        <v>124</v>
       </c>
       <c r="F52" s="26">
-        <v>185.00630000000001</v>
+        <v>187.9725</v>
       </c>
       <c r="G52" s="32">
-        <v>184.7724</v>
+        <v>187.81190000000001</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B53" s="12">
         <v>17112018</v>
@@ -2573,153 +2625,155 @@
         <v>910</v>
       </c>
       <c r="E53" s="12">
-        <f>45.5+58+25</f>
-        <v>128.5</v>
+        <f>47+35.5+42.66</f>
+        <v>125.16</v>
       </c>
       <c r="F53" s="26">
-        <v>184.77180000000001</v>
+        <v>183.6551</v>
       </c>
       <c r="G53" s="32">
-        <v>184.60230000000001</v>
+        <v>183.49359999999999</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="B54" s="12">
-        <v>18112018</v>
+        <v>17112018</v>
       </c>
       <c r="C54" s="24">
-        <v>5.859027777776646</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D54" s="12">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="E54" s="12">
-        <f>42+25</f>
-        <v>67</v>
+        <f>32.5+28.2</f>
+        <v>60.7</v>
       </c>
       <c r="F54" s="26">
-        <v>184.60489999999999</v>
+        <v>188.22</v>
       </c>
       <c r="G54" s="32">
-        <v>184.51650000000001</v>
+        <v>188.15190000000001</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="B55" s="12">
-        <v>19112018</v>
+        <v>17112018</v>
       </c>
       <c r="C55" s="24">
-        <v>6.8395833333343035</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D55" s="12">
-        <v>839</v>
+        <v>910</v>
       </c>
       <c r="E55" s="12">
-        <v>44.5</v>
+        <f>27.5+34</f>
+        <v>61.5</v>
       </c>
       <c r="F55" s="26">
-        <v>184.51320000000001</v>
+        <v>184.8306</v>
       </c>
       <c r="G55" s="32">
-        <v>184.45490000000001</v>
+        <v>184.76439999999999</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B56" s="12">
-        <v>21112018</v>
+        <v>17112018</v>
       </c>
       <c r="C56" s="24">
-        <v>8.9166666666642413</v>
+        <v>4.8611111111094942</v>
       </c>
       <c r="D56" s="12">
-        <v>1030</v>
+        <v>910</v>
       </c>
       <c r="E56" s="12">
-        <v>52</v>
+        <f>30+31</f>
+        <v>61</v>
       </c>
       <c r="F56" s="26">
-        <v>184.45949999999999</v>
+        <v>183.67490000000001</v>
       </c>
       <c r="G56" s="32">
-        <v>184.39500000000001</v>
+        <v>183.6079</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B57" s="12">
-        <v>23112018</v>
+        <v>18112018</v>
       </c>
       <c r="C57" s="24">
-        <v>10.878472222218988</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D57" s="12">
-        <v>935</v>
+        <v>907</v>
       </c>
       <c r="E57" s="12">
-        <v>33.1</v>
+        <v>7.8</v>
       </c>
       <c r="F57" s="26">
-        <v>184.39879999999999</v>
+        <v>183.16909999999999</v>
       </c>
       <c r="G57" s="32">
-        <v>184.35890000000001</v>
+        <v>183.16</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="B58" s="12">
-        <v>25112018</v>
+        <v>18112018</v>
       </c>
       <c r="C58" s="24">
-        <v>13.125</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D58" s="12">
-        <v>1530</v>
+        <v>907</v>
       </c>
       <c r="E58" s="12">
-        <v>25</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F58" s="26">
-        <v>184.3579</v>
+        <v>183.78399999999999</v>
       </c>
       <c r="G58" s="32">
-        <v>184.32740000000001</v>
+        <v>183.7731</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="B59" s="12">
-        <v>28112018</v>
+        <v>18112018</v>
       </c>
       <c r="C59" s="24">
-        <v>15.854166666664241</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D59" s="12">
-        <v>900</v>
+        <v>907</v>
       </c>
       <c r="E59" s="12">
-        <v>22.66</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F59" s="26">
-        <v>184.32679999999999</v>
+        <v>183.64330000000001</v>
       </c>
       <c r="G59" s="32">
-        <v>184.2988</v>
+        <v>183.63380000000001</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -2727,231 +2781,236 @@
         <v>40</v>
       </c>
       <c r="B60" s="12">
-        <v>1122018</v>
+        <v>18112018</v>
       </c>
       <c r="C60" s="24">
-        <v>18.909722222218988</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D60" s="12">
-        <v>1020</v>
+        <v>907</v>
       </c>
       <c r="E60" s="12">
-        <v>20.100000000000001</v>
+        <f>42+25</f>
+        <v>67</v>
       </c>
       <c r="F60" s="26">
-        <v>184.29990000000001</v>
+        <v>184.60489999999999</v>
       </c>
       <c r="G60" s="32">
-        <v>184.2747</v>
+        <v>184.51650000000001</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B61" s="12">
-        <v>5122018</v>
+        <v>18112018</v>
       </c>
       <c r="C61" s="24">
-        <v>22.861111111109494</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D61" s="12">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="E61" s="12">
-        <v>21.6</v>
+        <f>29.5+34</f>
+        <v>63.5</v>
       </c>
       <c r="F61" s="26">
-        <v>184.26939999999999</v>
+        <v>187.8126</v>
       </c>
       <c r="G61" s="32">
-        <v>184.2433</v>
+        <v>187.7285</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B62" s="12">
-        <v>9122018</v>
+        <v>18112018</v>
       </c>
       <c r="C62" s="24">
-        <v>27.145833333328483</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D62" s="12">
-        <v>1600</v>
+        <v>907</v>
       </c>
       <c r="E62" s="12">
-        <v>21.1</v>
+        <f>30+35</f>
+        <v>65</v>
       </c>
       <c r="F62" s="26">
-        <v>184.24299999999999</v>
+        <v>183.49600000000001</v>
       </c>
       <c r="G62" s="32">
-        <v>184.21700000000001</v>
+        <v>183.4102</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="B63" s="12">
-        <v>12112018</v>
+        <v>18112018</v>
       </c>
       <c r="C63" s="24">
-        <v>0</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D63" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E63"/>
+        <v>907</v>
+      </c>
+      <c r="E63" s="12">
+        <v>38</v>
+      </c>
+      <c r="F63" s="26">
+        <v>188.15549999999999</v>
+      </c>
       <c r="G63" s="32">
-        <v>188.50425000000001</v>
+        <v>188.113</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B64" s="12">
-        <v>13112018</v>
+        <v>18112018</v>
       </c>
       <c r="C64" s="24">
-        <v>0.84027777777373558</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D64" s="12">
-        <v>840</v>
+        <v>907</v>
       </c>
       <c r="E64" s="12">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F64" s="26">
-        <v>188.5035</v>
+        <v>184.76730000000001</v>
       </c>
       <c r="G64" s="32">
-        <v>188.4641</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>184.72450000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B65" s="12">
-        <v>14112018</v>
+        <v>18112018</v>
       </c>
       <c r="C65" s="24">
-        <v>1.84375</v>
+        <v>5.859027777776646</v>
       </c>
       <c r="D65" s="12">
-        <v>845</v>
+        <v>907</v>
       </c>
       <c r="E65" s="12">
-        <v>48</v>
+        <v>38.75</v>
       </c>
       <c r="F65" s="26">
-        <v>188.46549999999999</v>
+        <v>183.61019999999999</v>
       </c>
       <c r="G65" s="32">
-        <v>188.4084</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.56649999999999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="B66" s="12">
-        <v>15112018</v>
+        <v>19112018</v>
       </c>
       <c r="C66" s="24">
-        <v>2.8506944444452529</v>
+        <v>6.8395833333343035</v>
       </c>
       <c r="D66" s="12">
-        <v>855</v>
+        <v>839</v>
       </c>
       <c r="E66" s="12">
-        <f>57+29.6+44.5+36.6</f>
-        <v>167.7</v>
+        <v>7.5</v>
       </c>
       <c r="F66" s="26">
-        <v>188.4049</v>
+        <v>183.15600000000001</v>
       </c>
       <c r="G66" s="32">
-        <v>188.2022</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.1473</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B67" s="12">
-        <v>16112018</v>
+        <v>19112018</v>
       </c>
       <c r="C67" s="24">
-        <v>3.8090277777737356</v>
+        <v>6.8395833333343035</v>
       </c>
       <c r="D67" s="12">
-        <v>755</v>
+        <v>839</v>
       </c>
       <c r="E67" s="12">
-        <f>38+52+42+50</f>
-        <v>182</v>
+        <v>8.1</v>
       </c>
       <c r="F67" s="26">
-        <v>188.20359999999999</v>
+        <v>183.77019999999999</v>
       </c>
       <c r="G67" s="32">
-        <v>187.97470000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.7604</v>
+      </c>
+      <c r="H67" s="25"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="B68" s="12">
-        <v>17112018</v>
+        <v>19112018</v>
       </c>
       <c r="C68" s="24">
-        <v>4.8611111111094942</v>
+        <v>6.8395833333343035</v>
       </c>
       <c r="D68" s="12">
-        <v>910</v>
+        <v>839</v>
       </c>
       <c r="E68" s="12">
-        <f>48+23+53</f>
-        <v>124</v>
+        <v>7.2</v>
       </c>
       <c r="F68" s="26">
-        <v>187.9725</v>
+        <v>183.63130000000001</v>
       </c>
       <c r="G68" s="32">
-        <v>187.81190000000001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.62280000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B69" s="12">
-        <v>18112018</v>
+        <v>19112018</v>
       </c>
       <c r="C69" s="24">
-        <v>5.859027777776646</v>
+        <v>6.8395833333343035</v>
       </c>
       <c r="D69" s="12">
-        <v>907</v>
+        <v>839</v>
       </c>
       <c r="E69" s="12">
-        <f>29.5+34</f>
-        <v>63.5</v>
+        <v>44.5</v>
       </c>
       <c r="F69" s="26">
-        <v>187.8126</v>
+        <v>184.51320000000001</v>
       </c>
       <c r="G69" s="32">
-        <v>187.7285</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>184.45490000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>41</v>
       </c>
@@ -2974,376 +3033,377 @@
         <v>187.6705</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="12">
+        <v>19112018</v>
+      </c>
+      <c r="C71" s="24">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="D71" s="12">
+        <v>839</v>
+      </c>
+      <c r="E71" s="12">
+        <v>44</v>
+      </c>
+      <c r="F71" s="26">
+        <v>183.40639999999999</v>
+      </c>
+      <c r="G71" s="32">
+        <v>183.34950000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B72" s="12">
+        <v>19112018</v>
+      </c>
+      <c r="C72" s="24">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="D72" s="12">
+        <v>839</v>
+      </c>
+      <c r="E72" s="12">
+        <v>29.5</v>
+      </c>
+      <c r="F72" s="26">
+        <v>188.10890000000001</v>
+      </c>
+      <c r="G72" s="32">
+        <v>188.07589999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="12">
+        <v>19112018</v>
+      </c>
+      <c r="C73" s="24">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="D73" s="12">
+        <v>839</v>
+      </c>
+      <c r="E73" s="12">
+        <v>29</v>
+      </c>
+      <c r="F73" s="26">
+        <v>184.72069999999999</v>
+      </c>
+      <c r="G73" s="32">
+        <v>184.68860000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="12">
+        <v>19112018</v>
+      </c>
+      <c r="C74" s="24">
+        <v>6.8395833333343035</v>
+      </c>
+      <c r="D74" s="12">
+        <v>839</v>
+      </c>
+      <c r="E74" s="12">
+        <v>29</v>
+      </c>
+      <c r="F74" s="26">
+        <v>183.56319999999999</v>
+      </c>
+      <c r="G74" s="32">
+        <v>183.5308</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75" s="12">
+        <v>21112018</v>
+      </c>
+      <c r="C75" s="24">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="D75" s="12">
+        <v>1030</v>
+      </c>
+      <c r="E75" s="12">
+        <v>12.8</v>
+      </c>
+      <c r="F75" s="26">
+        <v>183.1523</v>
+      </c>
+      <c r="G75" s="32">
+        <v>183.13749999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" s="12">
+        <v>21112018</v>
+      </c>
+      <c r="C76" s="24">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="D76" s="12">
+        <v>1030</v>
+      </c>
+      <c r="E76" s="12">
+        <v>15</v>
+      </c>
+      <c r="F76" s="26">
+        <v>183.76429999999999</v>
+      </c>
+      <c r="G76" s="32">
+        <v>183.74770000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B77" s="12">
+        <v>21112018</v>
+      </c>
+      <c r="C77" s="24">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="D77" s="12">
+        <v>1030</v>
+      </c>
+      <c r="E77" s="12">
+        <v>13.1</v>
+      </c>
+      <c r="F77" s="26">
+        <v>183.62649999999999</v>
+      </c>
+      <c r="G77" s="32">
+        <v>183.61080000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B78" s="12">
+        <v>21112018</v>
+      </c>
+      <c r="C78" s="24">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="D78" s="12">
+        <v>1030</v>
+      </c>
+      <c r="E78" s="12">
+        <v>52</v>
+      </c>
+      <c r="F78" s="26">
+        <v>184.45949999999999</v>
+      </c>
+      <c r="G78" s="32">
+        <v>184.39500000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B71" s="12">
+      <c r="B79" s="12">
         <v>21112018</v>
       </c>
-      <c r="C71" s="24">
+      <c r="C79" s="24">
         <v>8.9166666666642413</v>
       </c>
-      <c r="D71" s="12">
+      <c r="D79" s="12">
         <v>1030</v>
       </c>
-      <c r="E71" s="12">
+      <c r="E79" s="12">
         <v>54.1</v>
       </c>
-      <c r="F71" s="26">
+      <c r="F79" s="26">
         <v>187.6746</v>
       </c>
-      <c r="G71" s="32">
+      <c r="G79" s="32">
         <v>187.60820000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B72" s="12">
-        <v>23112018</v>
-      </c>
-      <c r="C72" s="24">
-        <v>10.878472222218988</v>
-      </c>
-      <c r="D72" s="12">
-        <v>935</v>
-      </c>
-      <c r="E72" s="12">
-        <v>36.5</v>
-      </c>
-      <c r="F72" s="26">
-        <v>187.61199999999999</v>
-      </c>
-      <c r="G72" s="32">
-        <v>187.56800000000001</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B73" s="12">
-        <v>25112018</v>
-      </c>
-      <c r="C73" s="24">
-        <v>13.125</v>
-      </c>
-      <c r="D73" s="12">
-        <v>1530</v>
-      </c>
-      <c r="E73" s="12">
-        <v>24</v>
-      </c>
-      <c r="F73" s="31">
-        <v>187.5669</v>
-      </c>
-      <c r="G73" s="32">
-        <v>187.53749999999999</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B74" s="12">
-        <v>28112018</v>
-      </c>
-      <c r="C74" s="24">
-        <v>15.854166666664241</v>
-      </c>
-      <c r="D74" s="12">
-        <v>900</v>
-      </c>
-      <c r="E74" s="12">
-        <v>21.1</v>
-      </c>
-      <c r="F74" s="26">
-        <v>187.53630000000001</v>
-      </c>
-      <c r="G74" s="32">
-        <v>187.5093</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B75" s="12">
-        <v>1122018</v>
-      </c>
-      <c r="C75" s="24">
-        <v>18.909722222218988</v>
-      </c>
-      <c r="D75" s="12">
-        <v>1020</v>
-      </c>
-      <c r="E75" s="12">
-        <v>17.100000000000001</v>
-      </c>
-      <c r="F75" s="26">
-        <v>187.51130000000001</v>
-      </c>
-      <c r="G75" s="32">
-        <v>187.49029999999999</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B76" s="12">
-        <v>5122018</v>
-      </c>
-      <c r="C76" s="24">
-        <v>22.861111111109494</v>
-      </c>
-      <c r="D76" s="12">
-        <v>910</v>
-      </c>
-      <c r="E76" s="12">
-        <v>18.5</v>
-      </c>
-      <c r="F76" s="26">
-        <v>187.4854</v>
-      </c>
-      <c r="G76" s="32">
-        <v>187.46270000000001</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B77" s="12">
-        <v>9122018</v>
-      </c>
-      <c r="C77" s="24">
-        <v>27.145833333328483</v>
-      </c>
-      <c r="D77" s="12">
-        <v>1600</v>
-      </c>
-      <c r="E77" s="12">
-        <v>20.5</v>
-      </c>
-      <c r="F77" s="26">
-        <v>187.46119999999999</v>
-      </c>
-      <c r="G77" s="32">
-        <v>187.43680000000001</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B78" s="12">
-        <v>12112018</v>
-      </c>
-      <c r="C78" s="24">
-        <v>0</v>
-      </c>
-      <c r="D78" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E78"/>
-      <c r="G78" s="32">
-        <v>184.17580000000001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B79" s="12">
-        <v>13112018</v>
-      </c>
-      <c r="C79" s="24">
-        <v>0.84027777777373558</v>
-      </c>
-      <c r="D79" s="12">
-        <v>840</v>
-      </c>
-      <c r="E79" s="12">
-        <v>28.5</v>
-      </c>
-      <c r="F79" s="26">
-        <v>184.1746</v>
-      </c>
-      <c r="G79" s="32">
-        <v>184.13939999999999</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
         <v>42</v>
       </c>
       <c r="B80" s="12">
-        <v>14112018</v>
+        <v>21112018</v>
       </c>
       <c r="C80" s="24">
-        <v>1.84375</v>
+        <v>8.9166666666642413</v>
       </c>
       <c r="D80" s="12">
-        <v>845</v>
+        <v>1030</v>
       </c>
       <c r="E80" s="12">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F80" s="26">
-        <v>184.1405</v>
+        <v>183.3526</v>
       </c>
       <c r="G80" s="32">
-        <v>184.08320000000001</v>
+        <v>183.28970000000001</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B81" s="12">
-        <v>15112018</v>
+        <v>21112018</v>
       </c>
       <c r="C81" s="24">
-        <v>2.8506944444452529</v>
+        <v>8.9166666666642413</v>
       </c>
       <c r="D81" s="12">
-        <v>855</v>
+        <v>1030</v>
       </c>
       <c r="E81" s="12">
-        <f>35+51.6+37+40</f>
-        <v>163.6</v>
+        <v>41</v>
       </c>
       <c r="F81" s="26">
-        <v>184.0796</v>
+        <v>188.08009999999999</v>
       </c>
       <c r="G81" s="32">
-        <v>183.88130000000001</v>
+        <v>188.0343</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B82" s="12">
-        <v>16112018</v>
+        <v>21112018</v>
       </c>
       <c r="C82" s="24">
-        <v>3.8090277777737356</v>
+        <v>8.9166666666642413</v>
       </c>
       <c r="D82" s="12">
-        <v>755</v>
+        <v>1030</v>
       </c>
       <c r="E82" s="12">
-        <f>41+47.5+50+40.25</f>
-        <v>178.75</v>
+        <v>41</v>
       </c>
       <c r="F82" s="26">
-        <v>183.88200000000001</v>
+        <v>184.6926</v>
       </c>
       <c r="G82" s="32">
-        <v>183.6568</v>
+        <v>184.64609999999999</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="12">
+        <v>21112018</v>
+      </c>
+      <c r="C83" s="24">
+        <v>8.9166666666642413</v>
+      </c>
+      <c r="D83" s="12">
+        <v>1030</v>
+      </c>
+      <c r="E83" s="12">
         <v>42</v>
       </c>
-      <c r="B83" s="12">
-        <v>17112018</v>
-      </c>
-      <c r="C83" s="24">
-        <v>4.8611111111094942</v>
-      </c>
-      <c r="D83" s="12">
-        <v>910</v>
-      </c>
-      <c r="E83" s="12">
-        <f>47+35.5+42.66</f>
-        <v>125.16</v>
-      </c>
       <c r="F83" s="26">
-        <v>183.6551</v>
+        <v>183.5341</v>
       </c>
       <c r="G83" s="32">
-        <v>183.49359999999999</v>
+        <v>183.48779999999999</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B84" s="12">
-        <v>18112018</v>
+        <v>23112018</v>
       </c>
       <c r="C84" s="24">
-        <v>5.859027777776646</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D84" s="12">
-        <v>907</v>
+        <v>935</v>
       </c>
       <c r="E84" s="12">
-        <f>30+35</f>
-        <v>65</v>
+        <v>11</v>
       </c>
       <c r="F84" s="26">
-        <v>183.49600000000001</v>
+        <v>183.1396</v>
       </c>
       <c r="G84" s="32">
-        <v>183.4102</v>
+        <v>183.1276</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B85" s="12">
-        <v>19112018</v>
+        <v>23112018</v>
       </c>
       <c r="C85" s="24">
-        <v>6.8395833333343035</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D85" s="12">
-        <v>839</v>
+        <v>935</v>
       </c>
       <c r="E85" s="12">
-        <v>44</v>
+        <v>10.75</v>
       </c>
       <c r="F85" s="26">
-        <v>183.40639999999999</v>
+        <v>183.75149999999999</v>
       </c>
       <c r="G85" s="32">
-        <v>183.34950000000001</v>
+        <v>183.73779999999999</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B86" s="12">
-        <v>21112018</v>
+        <v>23112018</v>
       </c>
       <c r="C86" s="24">
-        <v>8.9166666666642413</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D86" s="12">
-        <v>1030</v>
+        <v>935</v>
       </c>
       <c r="E86" s="12">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="F86" s="26">
-        <v>183.3526</v>
+        <v>183.61439999999999</v>
       </c>
       <c r="G86" s="32">
-        <v>183.28970000000001</v>
+        <v>183.6018</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B87" s="12">
         <v>23112018</v>
@@ -3358,33 +3418,33 @@
         <v>33.1</v>
       </c>
       <c r="F87" s="26">
-        <v>183.29329999999999</v>
+        <v>184.39879999999999</v>
       </c>
       <c r="G87" s="32">
-        <v>183.25309999999999</v>
+        <v>184.35890000000001</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B88" s="12">
-        <v>25112018</v>
+        <v>23112018</v>
       </c>
       <c r="C88" s="24">
-        <v>13.125</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D88" s="12">
-        <v>1530</v>
+        <v>935</v>
       </c>
       <c r="E88" s="12">
-        <v>25</v>
+        <v>36.5</v>
       </c>
       <c r="F88" s="26">
-        <v>183.2527</v>
+        <v>187.61199999999999</v>
       </c>
       <c r="G88" s="32">
-        <v>183.22219999999999</v>
+        <v>187.56800000000001</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3392,349 +3452,349 @@
         <v>42</v>
       </c>
       <c r="B89" s="12">
-        <v>28112018</v>
+        <v>23112018</v>
       </c>
       <c r="C89" s="24">
-        <v>15.854166666664241</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D89" s="12">
-        <v>900</v>
+        <v>935</v>
       </c>
       <c r="E89" s="12">
-        <v>24.2</v>
+        <v>33.1</v>
       </c>
       <c r="F89" s="26">
-        <v>183.22040000000001</v>
+        <v>183.29329999999999</v>
       </c>
       <c r="G89" s="32">
-        <v>183.19300000000001</v>
+        <v>183.25309999999999</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B90" s="12">
-        <v>1122018</v>
+        <v>23112018</v>
       </c>
       <c r="C90" s="24">
-        <v>18.909722222218988</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D90" s="12">
-        <v>1020</v>
+        <v>935</v>
       </c>
       <c r="E90" s="12">
-        <v>20.100000000000001</v>
+        <v>30</v>
       </c>
       <c r="F90" s="26">
-        <v>183.19380000000001</v>
+        <v>188.03899999999999</v>
       </c>
       <c r="G90" s="32">
-        <v>183.16909999999999</v>
+        <v>188.0061</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="B91" s="12">
-        <v>5122018</v>
+        <v>23112018</v>
       </c>
       <c r="C91" s="24">
-        <v>22.861111111109494</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D91" s="12">
-        <v>910</v>
+        <v>935</v>
       </c>
       <c r="E91" s="12">
-        <v>21</v>
+        <v>28.5</v>
       </c>
       <c r="F91" s="26">
-        <v>183.16380000000001</v>
+        <v>184.65020000000001</v>
       </c>
       <c r="G91" s="32">
-        <v>183.1387</v>
+        <v>184.6189</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="B92" s="12">
-        <v>9122018</v>
+        <v>23112018</v>
       </c>
       <c r="C92" s="24">
-        <v>27.145833333328483</v>
+        <v>10.878472222218988</v>
       </c>
       <c r="D92" s="12">
-        <v>1600</v>
+        <v>935</v>
       </c>
       <c r="E92" s="12">
-        <v>21</v>
+        <v>29.8</v>
       </c>
       <c r="F92" s="26">
-        <v>183.13749999999999</v>
+        <v>183.4923</v>
       </c>
       <c r="G92" s="32">
-        <v>183.11179999999999</v>
+        <v>183.46</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B93" s="12">
-        <v>12112018</v>
+        <v>25112018</v>
       </c>
       <c r="C93" s="24">
-        <v>0</v>
+        <v>13.125</v>
       </c>
       <c r="D93" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E93"/>
+        <v>1530</v>
+      </c>
+      <c r="E93" s="12">
+        <v>12.66</v>
+      </c>
+      <c r="F93" s="26">
+        <v>183.12700000000001</v>
+      </c>
       <c r="G93" s="32">
-        <v>188.87815000000001</v>
+        <v>183.11240000000001</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B94" s="12">
-        <v>13112018</v>
+        <v>25112018</v>
       </c>
       <c r="C94" s="24">
-        <v>0.84027777777373558</v>
+        <v>13.125</v>
       </c>
       <c r="D94" s="12">
-        <v>840</v>
+        <v>1530</v>
       </c>
       <c r="E94" s="12">
-        <f>50+50+38</f>
-        <v>138</v>
-      </c>
-      <c r="F94" s="26">
-        <v>188.87790000000001</v>
+        <v>13.33</v>
+      </c>
+      <c r="F94" s="30">
+        <v>183.73650000000001</v>
       </c>
       <c r="G94" s="32">
-        <v>188.71129999999999</v>
+        <v>183.7217</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="B95" s="12">
-        <v>14112018</v>
+        <v>25112018</v>
       </c>
       <c r="C95" s="24">
-        <v>1.84375</v>
+        <v>13.125</v>
       </c>
       <c r="D95" s="12">
-        <v>845</v>
+        <v>1530</v>
       </c>
       <c r="E95" s="12">
-        <f>53+37+31.6+51.3</f>
-        <v>172.89999999999998</v>
+        <v>12.33</v>
       </c>
       <c r="F95" s="26">
-        <v>188.71180000000001</v>
+        <v>183.6009</v>
       </c>
       <c r="G95" s="32">
-        <v>188.5119</v>
+        <v>183.58670000000001</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="B96" s="12">
-        <v>15112018</v>
+        <v>25112018</v>
       </c>
       <c r="C96" s="24">
-        <v>2.8506944444452529</v>
+        <v>13.125</v>
       </c>
       <c r="D96" s="12">
-        <v>855</v>
+        <v>1530</v>
       </c>
       <c r="E96" s="12">
-        <f>35.5+45.25+35.25+49.5</f>
-        <v>165.5</v>
+        <v>25</v>
       </c>
       <c r="F96" s="26">
-        <v>188.50700000000001</v>
+        <v>184.3579</v>
       </c>
       <c r="G96" s="32">
-        <v>188.328</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+        <v>184.32740000000001</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B97" s="12">
-        <v>16112018</v>
+        <v>25112018</v>
       </c>
       <c r="C97" s="24">
-        <v>3.8090277777737356</v>
+        <v>13.125</v>
       </c>
       <c r="D97" s="12">
-        <v>755</v>
+        <v>1530</v>
       </c>
       <c r="E97" s="12">
-        <f>29.66+21+22+28.5</f>
-        <v>101.16</v>
-      </c>
-      <c r="F97" s="26">
-        <v>188.3279</v>
+        <v>24</v>
+      </c>
+      <c r="F97" s="31">
+        <v>187.5669</v>
       </c>
       <c r="G97" s="32">
-        <v>188.22149999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>187.53749999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B98" s="12">
-        <v>17112018</v>
+        <v>25112018</v>
       </c>
       <c r="C98" s="24">
-        <v>4.8611111111094942</v>
+        <v>13.125</v>
       </c>
       <c r="D98" s="12">
-        <v>910</v>
+        <v>1530</v>
       </c>
       <c r="E98" s="12">
-        <f>32.5+28.2</f>
-        <v>60.7</v>
+        <v>25</v>
       </c>
       <c r="F98" s="26">
-        <v>188.22</v>
+        <v>183.2527</v>
       </c>
       <c r="G98" s="32">
-        <v>188.15190000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.22219999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B99" s="12">
-        <v>18112018</v>
+        <v>25112018</v>
       </c>
       <c r="C99" s="24">
-        <v>5.859027777776646</v>
+        <v>13.125</v>
       </c>
       <c r="D99" s="12">
-        <v>907</v>
+        <v>1530</v>
       </c>
       <c r="E99" s="12">
-        <v>38</v>
+        <v>24.33</v>
       </c>
       <c r="F99" s="26">
-        <v>188.15549999999999</v>
+        <v>188.005</v>
       </c>
       <c r="G99" s="32">
-        <v>188.113</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>187.9777</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B100" s="12">
-        <v>19112018</v>
+        <v>25112018</v>
       </c>
       <c r="C100" s="24">
-        <v>6.8395833333343035</v>
+        <v>13.125</v>
       </c>
       <c r="D100" s="12">
-        <v>839</v>
+        <v>1530</v>
       </c>
       <c r="E100" s="12">
-        <v>29.5</v>
-      </c>
-      <c r="F100" s="26">
-        <v>188.10890000000001</v>
+        <v>24.5</v>
+      </c>
+      <c r="F100" s="31">
+        <v>184.6164</v>
       </c>
       <c r="G100" s="32">
-        <v>188.07589999999999</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>184.58949999999999</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B101" s="12">
-        <v>21112018</v>
+        <v>25112018</v>
       </c>
       <c r="C101" s="24">
-        <v>8.9166666666642413</v>
+        <v>13.125</v>
       </c>
       <c r="D101" s="12">
-        <v>1030</v>
+        <v>1530</v>
       </c>
       <c r="E101" s="12">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="F101" s="26">
-        <v>188.08009999999999</v>
+        <v>183.45820000000001</v>
       </c>
       <c r="G101" s="32">
-        <v>188.0343</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.4308</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B102" s="12">
-        <v>23112018</v>
+        <v>28112018</v>
       </c>
       <c r="C102" s="24">
-        <v>10.878472222218988</v>
+        <v>15.854166666664241</v>
       </c>
       <c r="D102" s="12">
-        <v>935</v>
+        <v>900</v>
       </c>
       <c r="E102" s="12">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F102" s="26">
-        <v>188.03899999999999</v>
+        <v>183.11019999999999</v>
       </c>
       <c r="G102" s="32">
-        <v>188.0061</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.09610000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="B103" s="12">
-        <v>25112018</v>
+        <v>28112018</v>
       </c>
       <c r="C103" s="24">
-        <v>13.125</v>
+        <v>15.854166666664241</v>
       </c>
       <c r="D103" s="12">
-        <v>1530</v>
+        <v>900</v>
       </c>
       <c r="E103" s="12">
-        <v>24.33</v>
+        <v>13</v>
       </c>
       <c r="F103" s="26">
-        <v>188.005</v>
+        <v>183.721</v>
       </c>
       <c r="G103" s="32">
-        <v>187.9777</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.70490000000001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="12" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="B104" s="12">
         <v>28112018</v>
@@ -3746,311 +3806,313 @@
         <v>900</v>
       </c>
       <c r="E104" s="12">
+        <v>12.33</v>
+      </c>
+      <c r="F104" s="26">
+        <v>183.5848</v>
+      </c>
+      <c r="G104" s="32">
+        <v>183.57140000000001</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B105" s="12">
+        <v>28112018</v>
+      </c>
+      <c r="C105" s="24">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="D105" s="12">
+        <v>900</v>
+      </c>
+      <c r="E105" s="12">
+        <v>22.66</v>
+      </c>
+      <c r="F105" s="26">
+        <v>184.32679999999999</v>
+      </c>
+      <c r="G105" s="32">
+        <v>184.2988</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B106" s="12">
+        <v>28112018</v>
+      </c>
+      <c r="C106" s="24">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="D106" s="12">
+        <v>900</v>
+      </c>
+      <c r="E106" s="12">
+        <v>21.1</v>
+      </c>
+      <c r="F106" s="26">
+        <v>187.53630000000001</v>
+      </c>
+      <c r="G106" s="32">
+        <v>187.5093</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B107" s="12">
+        <v>28112018</v>
+      </c>
+      <c r="C107" s="24">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="D107" s="12">
+        <v>900</v>
+      </c>
+      <c r="E107" s="12">
+        <v>24.2</v>
+      </c>
+      <c r="F107" s="26">
+        <v>183.22040000000001</v>
+      </c>
+      <c r="G107" s="32">
+        <v>183.19300000000001</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B108" s="12">
+        <v>28112018</v>
+      </c>
+      <c r="C108" s="24">
+        <v>15.854166666664241</v>
+      </c>
+      <c r="D108" s="12">
+        <v>900</v>
+      </c>
+      <c r="E108" s="12">
         <v>23</v>
       </c>
-      <c r="F104" s="26">
+      <c r="F108" s="26">
         <v>187.97730000000001</v>
       </c>
-      <c r="G104" s="32">
+      <c r="G108" s="32">
         <v>187.95089999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B105" s="12">
-        <v>1122018</v>
-      </c>
-      <c r="C105" s="24">
-        <v>18.909722222218988</v>
-      </c>
-      <c r="D105" s="12">
-        <v>1020</v>
-      </c>
-      <c r="E105" s="12">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="F105" s="26">
-        <v>187.9522</v>
-      </c>
-      <c r="G105" s="32">
-        <v>187.93039999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B106" s="12">
-        <v>5122018</v>
-      </c>
-      <c r="C106" s="24">
-        <v>22.861111111109494</v>
-      </c>
-      <c r="D106" s="12">
-        <v>910</v>
-      </c>
-      <c r="E106" s="12">
-        <v>20.6</v>
-      </c>
-      <c r="F106" s="26">
-        <v>187.92500000000001</v>
-      </c>
-      <c r="G106" s="32">
-        <v>187.9008</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B107" s="12">
-        <v>9122018</v>
-      </c>
-      <c r="C107" s="24">
-        <v>27.145833333328483</v>
-      </c>
-      <c r="D107" s="12">
-        <v>1600</v>
-      </c>
-      <c r="E107" s="12">
-        <v>19.3</v>
-      </c>
-      <c r="F107" s="26">
-        <v>187.9007</v>
-      </c>
-      <c r="G107" s="32">
-        <v>187.87819999999999</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B108" s="12">
-        <v>12112018</v>
-      </c>
-      <c r="C108" s="24">
-        <v>0</v>
-      </c>
-      <c r="D108" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E108"/>
-      <c r="G108" s="32">
-        <v>185.49180000000001</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B109" s="12">
-        <v>13112018</v>
+        <v>28112018</v>
       </c>
       <c r="C109" s="24">
-        <v>0.84027777777373558</v>
+        <v>15.854166666664241</v>
       </c>
       <c r="D109" s="12">
-        <v>840</v>
+        <v>900</v>
       </c>
       <c r="E109" s="12">
-        <v>135.5</v>
+        <v>22.5</v>
       </c>
       <c r="F109" s="26">
-        <v>185.49119999999999</v>
+        <v>184.58760000000001</v>
       </c>
       <c r="G109" s="32">
-        <v>185.3244</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>184.56100000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B110" s="12">
-        <v>14112018</v>
+        <v>28112018</v>
       </c>
       <c r="C110" s="24">
-        <v>1.84375</v>
+        <v>15.854166666664241</v>
       </c>
       <c r="D110" s="12">
-        <v>845</v>
+        <v>900</v>
       </c>
       <c r="E110" s="12">
-        <f>30+56.3+44+44</f>
-        <v>174.3</v>
+        <v>24.66</v>
       </c>
       <c r="F110" s="26">
-        <v>185.3254</v>
+        <v>183.4297</v>
       </c>
       <c r="G110" s="32">
-        <v>185.12260000000001</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.40209999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B111" s="12">
-        <v>15112018</v>
+        <v>1122018</v>
       </c>
       <c r="C111" s="24">
-        <v>2.8506944444452529</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D111" s="12">
-        <v>855</v>
+        <v>1020</v>
       </c>
       <c r="E111" s="12">
-        <f>48.5+37.5+40+42</f>
-        <v>168</v>
+        <v>11</v>
       </c>
       <c r="F111" s="26">
-        <v>185.11920000000001</v>
+        <v>183.09690000000001</v>
       </c>
       <c r="G111" s="32">
-        <v>184.93819999999999</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+        <v>183.08510000000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B112" s="12">
-        <v>16112018</v>
+        <v>1122018</v>
       </c>
       <c r="C112" s="24">
-        <v>3.8090277777737356</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D112" s="12">
-        <v>755</v>
+        <v>1020</v>
       </c>
       <c r="E112" s="12">
-        <f>53+45</f>
-        <v>98</v>
+        <v>11</v>
       </c>
       <c r="F112" s="26">
-        <v>184.9402</v>
+        <v>183.70509999999999</v>
       </c>
       <c r="G112" s="32">
-        <v>184.833</v>
-      </c>
+        <v>183.69239999999999</v>
+      </c>
+      <c r="H112" s="25"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B113" s="12">
-        <v>17112018</v>
+        <v>1122018</v>
       </c>
       <c r="C113" s="24">
-        <v>4.8611111111094942</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D113" s="12">
-        <v>910</v>
+        <v>1020</v>
       </c>
       <c r="E113" s="12">
-        <f>27.5+34</f>
-        <v>61.5</v>
+        <v>11</v>
       </c>
       <c r="F113" s="26">
-        <v>184.8306</v>
+        <v>183.5727</v>
       </c>
       <c r="G113" s="32">
-        <v>184.76439999999999</v>
+        <v>183.5592</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B114" s="12">
-        <v>18112018</v>
+        <v>1122018</v>
       </c>
       <c r="C114" s="24">
-        <v>5.859027777776646</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D114" s="12">
-        <v>907</v>
+        <v>1020</v>
       </c>
       <c r="E114" s="12">
-        <v>38</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F114" s="26">
-        <v>184.76730000000001</v>
+        <v>184.29990000000001</v>
       </c>
       <c r="G114" s="32">
-        <v>184.72450000000001</v>
+        <v>184.2747</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B115" s="12">
-        <v>19112018</v>
+        <v>1122018</v>
       </c>
       <c r="C115" s="24">
-        <v>6.8395833333343035</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D115" s="12">
-        <v>839</v>
+        <v>1020</v>
       </c>
       <c r="E115" s="12">
-        <v>29</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F115" s="26">
-        <v>184.72069999999999</v>
+        <v>187.51130000000001</v>
       </c>
       <c r="G115" s="32">
-        <v>184.68860000000001</v>
+        <v>187.49029999999999</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B116" s="12">
-        <v>21112018</v>
+        <v>1122018</v>
       </c>
       <c r="C116" s="24">
-        <v>8.9166666666642413</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D116" s="12">
-        <v>1030</v>
+        <v>1020</v>
       </c>
       <c r="E116" s="12">
-        <v>41</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F116" s="26">
-        <v>184.6926</v>
+        <v>183.19380000000001</v>
       </c>
       <c r="G116" s="32">
-        <v>184.64609999999999</v>
+        <v>183.16909999999999</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B117" s="12">
-        <v>23112018</v>
+        <v>1122018</v>
       </c>
       <c r="C117" s="24">
-        <v>10.878472222218988</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D117" s="12">
-        <v>935</v>
+        <v>1020</v>
       </c>
       <c r="E117" s="12">
-        <v>28.5</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="F117" s="26">
-        <v>184.65020000000001</v>
+        <v>187.9522</v>
       </c>
       <c r="G117" s="32">
-        <v>184.6189</v>
+        <v>187.93039999999999</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4058,73 +4120,73 @@
         <v>9</v>
       </c>
       <c r="B118" s="12">
-        <v>25112018</v>
+        <v>1122018</v>
       </c>
       <c r="C118" s="24">
-        <v>13.125</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D118" s="12">
-        <v>1530</v>
+        <v>1020</v>
       </c>
       <c r="E118" s="12">
-        <v>24.5</v>
-      </c>
-      <c r="F118" s="31">
-        <v>184.6164</v>
+        <v>19</v>
+      </c>
+      <c r="F118" s="26">
+        <v>184.56370000000001</v>
       </c>
       <c r="G118" s="32">
-        <v>184.58949999999999</v>
+        <v>184.5419</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B119" s="12">
-        <v>28112018</v>
+        <v>1122018</v>
       </c>
       <c r="C119" s="24">
-        <v>15.854166666664241</v>
+        <v>18.909722222218988</v>
       </c>
       <c r="D119" s="12">
-        <v>900</v>
+        <v>1020</v>
       </c>
       <c r="E119" s="12">
-        <v>22.5</v>
+        <v>20</v>
       </c>
       <c r="F119" s="26">
-        <v>184.58760000000001</v>
+        <v>183.40299999999999</v>
       </c>
       <c r="G119" s="32">
-        <v>184.56100000000001</v>
+        <v>183.38030000000001</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="B120" s="12">
-        <v>1122018</v>
+        <v>5122018</v>
       </c>
       <c r="C120" s="24">
-        <v>18.909722222218988</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D120" s="12">
-        <v>1020</v>
+        <v>910</v>
       </c>
       <c r="E120" s="12">
-        <v>19</v>
+        <v>11.1</v>
       </c>
       <c r="F120" s="26">
-        <v>184.56370000000001</v>
+        <v>183.0789</v>
       </c>
       <c r="G120" s="32">
-        <v>184.5419</v>
+        <v>183.06549999999999</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
-        <v>9</v>
+        <v>58</v>
       </c>
       <c r="B121" s="12">
         <v>5122018</v>
@@ -4136,149 +4198,151 @@
         <v>910</v>
       </c>
       <c r="E121" s="12">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F121" s="26">
-        <v>184.53620000000001</v>
+        <v>183.6875</v>
       </c>
       <c r="G121" s="32">
-        <v>184.5128</v>
+        <v>183.67359999999999</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B122" s="12">
-        <v>9122018</v>
+        <v>5122018</v>
       </c>
       <c r="C122" s="24">
-        <v>27.145833333328483</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D122" s="12">
-        <v>1600</v>
+        <v>910</v>
       </c>
       <c r="E122" s="12">
-        <v>19.5</v>
+        <v>11.8</v>
       </c>
       <c r="F122" s="26">
-        <v>184.5112</v>
+        <v>183.55459999999999</v>
       </c>
       <c r="G122" s="32">
-        <v>184.48920000000001</v>
+        <v>183.53960000000001</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B123" s="12">
-        <v>12112018</v>
+        <v>5122018</v>
       </c>
       <c r="C123" s="24">
-        <v>0</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D123" s="12">
-        <v>1230</v>
-      </c>
-      <c r="E123"/>
+        <v>910</v>
+      </c>
+      <c r="E123" s="12">
+        <v>21.6</v>
+      </c>
+      <c r="F123" s="26">
+        <v>184.26939999999999</v>
+      </c>
       <c r="G123" s="32">
-        <v>184.33615</v>
+        <v>184.2433</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B124" s="12">
-        <v>13112018</v>
+        <v>5122018</v>
       </c>
       <c r="C124" s="24">
-        <v>0.84027777777373558</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D124" s="12">
-        <v>840</v>
+        <v>910</v>
       </c>
       <c r="E124" s="12">
-        <v>140.5</v>
+        <v>18.5</v>
       </c>
       <c r="F124" s="26">
-        <v>184.33600000000001</v>
+        <v>187.4854</v>
       </c>
       <c r="G124" s="32">
-        <v>184.16579999999999</v>
+        <v>187.46270000000001</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B125" s="12">
-        <v>14112018</v>
+        <v>5122018</v>
       </c>
       <c r="C125" s="24">
-        <v>1.84375</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D125" s="12">
-        <v>845</v>
+        <v>910</v>
       </c>
       <c r="E125" s="12">
-        <f>35.2+54.5+40.5+43.8</f>
-        <v>174</v>
+        <v>21</v>
       </c>
       <c r="F125" s="26">
-        <v>184.16659999999999</v>
+        <v>183.16380000000001</v>
       </c>
       <c r="G125" s="32">
-        <v>183.96469999999999</v>
+        <v>183.1387</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B126" s="12">
-        <v>15112018</v>
+        <v>5122018</v>
       </c>
       <c r="C126" s="24">
-        <v>2.8506944444452529</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D126" s="12">
-        <v>855</v>
+        <v>910</v>
       </c>
       <c r="E126" s="12">
-        <f>41+25.5+58+42</f>
-        <v>166.5</v>
+        <v>20.6</v>
       </c>
       <c r="F126" s="26">
-        <v>183.96039999999999</v>
+        <v>187.92500000000001</v>
       </c>
       <c r="G126" s="32">
-        <v>183.7807</v>
+        <v>187.9008</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B127" s="12">
-        <v>16112018</v>
+        <v>5122018</v>
       </c>
       <c r="C127" s="24">
-        <v>3.8090277777737356</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D127" s="12">
-        <v>755</v>
+        <v>910</v>
       </c>
       <c r="E127" s="12">
-        <f>50.25+49.5</f>
-        <v>99.75</v>
+        <v>21</v>
       </c>
       <c r="F127" s="26">
-        <v>183.78370000000001</v>
+        <v>184.53620000000001</v>
       </c>
       <c r="G127" s="32">
-        <v>183.67580000000001</v>
+        <v>184.5128</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -4286,207 +4350,206 @@
         <v>10</v>
       </c>
       <c r="B128" s="12">
-        <v>17112018</v>
+        <v>5122018</v>
       </c>
       <c r="C128" s="24">
-        <v>4.8611111111094942</v>
+        <v>22.861111111109494</v>
       </c>
       <c r="D128" s="12">
         <v>910</v>
       </c>
       <c r="E128" s="12">
-        <f>30+31</f>
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="F128" s="26">
-        <v>183.67490000000001</v>
+        <v>183.37479999999999</v>
       </c>
       <c r="G128" s="32">
-        <v>183.6079</v>
+        <v>183.35159999999999</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="B129" s="12">
-        <v>18112018</v>
+        <v>9122018</v>
       </c>
       <c r="C129" s="24">
-        <v>5.859027777776646</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D129" s="12">
-        <v>907</v>
+        <v>1600</v>
       </c>
       <c r="E129" s="12">
-        <v>38.75</v>
+        <v>13</v>
       </c>
       <c r="F129" s="26">
-        <v>183.61019999999999</v>
+        <v>183.06450000000001</v>
       </c>
       <c r="G129" s="32">
-        <v>183.56649999999999</v>
+        <v>183.04900000000001</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="B130" s="12">
-        <v>19112018</v>
+        <v>9122018</v>
       </c>
       <c r="C130" s="24">
-        <v>6.8395833333343035</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D130" s="12">
-        <v>839</v>
+        <v>1600</v>
       </c>
       <c r="E130" s="12">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F130" s="26">
-        <v>183.56319999999999</v>
+        <v>183.67250000000001</v>
       </c>
       <c r="G130" s="32">
-        <v>183.5308</v>
+        <v>183.65950000000001</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="B131" s="12">
-        <v>21112018</v>
+        <v>9122018</v>
       </c>
       <c r="C131" s="24">
-        <v>8.9166666666642413</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D131" s="12">
-        <v>1030</v>
+        <v>1600</v>
       </c>
       <c r="E131" s="12">
-        <v>42</v>
+        <v>11.6</v>
       </c>
       <c r="F131" s="26">
-        <v>183.5341</v>
+        <v>183.53899999999999</v>
       </c>
       <c r="G131" s="32">
-        <v>183.48779999999999</v>
+        <v>183.52619999999999</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B132" s="12">
-        <v>23112018</v>
+        <v>9122018</v>
       </c>
       <c r="C132" s="24">
-        <v>10.878472222218988</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D132" s="12">
-        <v>935</v>
+        <v>1600</v>
       </c>
       <c r="E132" s="12">
-        <v>29.8</v>
+        <v>21.1</v>
       </c>
       <c r="F132" s="26">
-        <v>183.4923</v>
+        <v>184.24299999999999</v>
       </c>
       <c r="G132" s="32">
-        <v>183.46</v>
+        <v>184.21700000000001</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B133" s="12">
-        <v>25112018</v>
+        <v>9122018</v>
       </c>
       <c r="C133" s="24">
-        <v>13.125</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D133" s="12">
-        <v>1530</v>
+        <v>1600</v>
       </c>
       <c r="E133" s="12">
-        <v>25</v>
+        <v>20.5</v>
       </c>
       <c r="F133" s="26">
-        <v>183.45820000000001</v>
+        <v>187.46119999999999</v>
       </c>
       <c r="G133" s="32">
-        <v>183.4308</v>
+        <v>187.43680000000001</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B134" s="12">
-        <v>28112018</v>
+        <v>9122018</v>
       </c>
       <c r="C134" s="24">
-        <v>15.854166666664241</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D134" s="12">
-        <v>900</v>
+        <v>1600</v>
       </c>
       <c r="E134" s="12">
-        <v>24.66</v>
+        <v>21</v>
       </c>
       <c r="F134" s="26">
-        <v>183.4297</v>
+        <v>183.13749999999999</v>
       </c>
       <c r="G134" s="32">
-        <v>183.40209999999999</v>
+        <v>183.11179999999999</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B135" s="12">
-        <v>1122018</v>
+        <v>9122018</v>
       </c>
       <c r="C135" s="24">
-        <v>18.909722222218988</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D135" s="12">
-        <v>1020</v>
+        <v>1600</v>
       </c>
       <c r="E135" s="12">
-        <v>20</v>
+        <v>19.3</v>
       </c>
       <c r="F135" s="26">
-        <v>183.40299999999999</v>
+        <v>187.9007</v>
       </c>
       <c r="G135" s="32">
-        <v>183.38030000000001</v>
+        <v>187.87819999999999</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B136" s="12">
-        <v>5122018</v>
+        <v>9122018</v>
       </c>
       <c r="C136" s="24">
-        <v>22.861111111109494</v>
+        <v>27.145833333328483</v>
       </c>
       <c r="D136" s="12">
-        <v>910</v>
+        <v>1600</v>
       </c>
       <c r="E136" s="12">
-        <v>21</v>
+        <v>19.5</v>
       </c>
       <c r="F136" s="26">
-        <v>183.37479999999999</v>
+        <v>184.5112</v>
       </c>
       <c r="G136" s="32">
-        <v>183.35159999999999</v>
+        <v>184.48920000000001</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -4513,6 +4576,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A3:H137">
+    <sortCondition ref="C3:C137"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -4522,7 +4588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -5189,10 +5255,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5273,8 +5339,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="10"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="19" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
@@ -5285,11 +5370,14 @@
     <row r="21" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D22" s="13"/>
-    </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D24" s="13"/>
+    <row r="22" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="13"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change UQ_gd.xlsx, run some code, add xCH4.plots.R to IlSBMP1 and correct the file for thermal hydrolysis after being saved wrong with IlSBMP1 code and change export_manipulated.R for BMP
</commit_message>
<xml_diff>
--- a/experiments/UQ2/gd/UQ2_GD.xlsx
+++ b/experiments/UQ2/gd/UQ2_GD.xlsx
@@ -253,7 +253,7 @@
     <t>Add 0 in volume for day 0</t>
   </si>
   <si>
-    <t>Add mas.init = mass.final instead of having empty rows to avoid NA problem in R</t>
+    <t>Add mass.init = mass.final instead of having empty rows to avoid NA problem in R for day 0</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,7 +4589,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5258,7 +5258,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add UQ2.gd table for supplementary
</commit_message>
<xml_diff>
--- a/experiments/UQ2/gd/UQ2_GD.xlsx
+++ b/experiments/UQ2/gd/UQ2_GD.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -254,6 +254,18 @@
   </si>
   <si>
     <t>Add mass.init = mass.final instead of having empty rows to avoid NA problem in R for day 0</t>
+  </si>
+  <si>
+    <t>conc.sub.vs</t>
+  </si>
+  <si>
+    <t>conc.ino.vs</t>
+  </si>
+  <si>
+    <t>Add conc.vs for inoc and sub</t>
+  </si>
+  <si>
+    <t>29.03.2019</t>
   </si>
 </sst>
 </file>
@@ -768,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,11 +791,13 @@
     <col min="1" max="2" width="11.85546875" style="14" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="11.85546875" style="14" customWidth="1"/>
-    <col min="10" max="1018" width="8.5703125" style="14"/>
+    <col min="10" max="12" width="8.5703125" style="14"/>
+    <col min="13" max="13" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="1018" width="8.5703125" style="14"/>
     <col min="1019" max="16384" width="9" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>24</v>
       </c>
@@ -818,7 +832,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -852,8 +866,14 @@
       <c r="K2" s="14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>57</v>
       </c>
@@ -886,8 +906,12 @@
       <c r="J3" s="20">
         <v>1.520558448048688</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="14">
+        <f>J3/(D3*1000)</f>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>58</v>
       </c>
@@ -920,8 +944,12 @@
       <c r="J4" s="20">
         <v>1.5210906168970626</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="14">
+        <f t="shared" ref="M4:M11" si="0">J4/(D4*1000)</f>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>59</v>
       </c>
@@ -941,11 +969,11 @@
         <v>0</v>
       </c>
       <c r="G5" s="27">
-        <f t="shared" ref="G5" si="0">SUM(D5:F5)</f>
+        <f t="shared" ref="G5" si="1">SUM(D5:F5)</f>
         <v>80.010999999999996</v>
       </c>
       <c r="H5" s="27">
-        <f t="shared" ref="H5" si="1">160-G5</f>
+        <f t="shared" ref="H5" si="2">160-G5</f>
         <v>79.989000000000004</v>
       </c>
       <c r="I5" s="20">
@@ -954,8 +982,12 @@
       <c r="J5" s="20">
         <v>1.5206914902607815</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>40</v>
       </c>
@@ -991,8 +1023,16 @@
       <c r="K6" s="20">
         <v>1.8340522384700824</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="14">
+        <f t="shared" ref="L5:L11" si="3">I6/(1000*E6)</f>
+        <v>9.7397515923315907E-4</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>41</v>
       </c>
@@ -1016,7 +1056,7 @@
         <v>80.86</v>
       </c>
       <c r="H7" s="27">
-        <f t="shared" ref="H7:H8" si="2">160-G8</f>
+        <f t="shared" ref="H7:H8" si="4">160-G8</f>
         <v>79.023600000000002</v>
       </c>
       <c r="I7" s="20">
@@ -1028,8 +1068,16 @@
       <c r="K7" s="20">
         <v>1.8345015054549394</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="14">
+        <f t="shared" si="3"/>
+        <v>9.7397515923315896E-4</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>42</v>
       </c>
@@ -1053,7 +1101,7 @@
         <v>80.976399999999998</v>
       </c>
       <c r="H8" s="27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>79.011600000000001</v>
       </c>
       <c r="I8" s="29">
@@ -1065,8 +1113,16 @@
       <c r="K8" s="20">
         <v>1.8324720373115726</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="14">
+        <f t="shared" si="3"/>
+        <v>9.7397515923315907E-4</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
@@ -1086,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="27">
-        <f t="shared" ref="G9:G10" si="3">SUM(D11:F11)</f>
+        <f t="shared" ref="G9:G10" si="5">SUM(D11:F11)</f>
         <v>80.988399999999999</v>
       </c>
       <c r="H9" s="27">
@@ -1102,8 +1158,16 @@
       <c r="K9" s="20">
         <v>1.9273905007195093</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="14">
+        <f t="shared" si="3"/>
+        <v>8.130054802589125E-4</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>9</v>
       </c>
@@ -1123,11 +1187,11 @@
         <v>0</v>
       </c>
       <c r="G10" s="27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H10" s="27">
-        <f t="shared" ref="H10:H11" si="4">160-G12</f>
+        <f t="shared" ref="H10:H11" si="6">160-G12</f>
         <v>160</v>
       </c>
       <c r="I10" s="29">
@@ -1139,8 +1203,16 @@
       <c r="K10" s="20">
         <v>1.9295953770092844</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="14">
+        <f t="shared" si="3"/>
+        <v>8.1300548025891261E-4</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>10</v>
       </c>
@@ -1164,7 +1236,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>160</v>
       </c>
       <c r="I11" s="29">
@@ -1176,13 +1248,21 @@
       <c r="K11" s="14">
         <v>1.9296922316001799</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="14">
+        <f t="shared" si="3"/>
+        <v>8.1300548025891239E-4</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
@@ -1191,7 +1271,7 @@
       <c r="I13" s="15"/>
       <c r="J13" s="21"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
@@ -1199,7 +1279,7 @@
       <c r="H14" s="16"/>
       <c r="I14" s="16"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1210,7 +1290,7 @@
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -5258,7 +5338,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5361,6 +5441,20 @@
         <v>73</v>
       </c>
     </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="19" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
     </row>

</xml_diff>

<commit_message>
Add table with round function
</commit_message>
<xml_diff>
--- a/experiments/UQ2/gd/UQ2_GD.xlsx
+++ b/experiments/UQ2/gd/UQ2_GD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855"/>
   </bookViews>
   <sheets>
     <sheet name="Setup_GD" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="80">
   <si>
     <t>id</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>29.03.2019</t>
+  </si>
+  <si>
+    <t>02.04.2019</t>
+  </si>
+  <si>
+    <t>Correct columns for conc.vs</t>
   </si>
 </sst>
 </file>
@@ -782,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,8 +913,8 @@
         <v>1.520558448048688</v>
       </c>
       <c r="M3" s="14">
-        <f>J3/(D3*1000)</f>
-        <v>1.9006030299093645E-5</v>
+        <f>(1000*J3)/D3</f>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -945,8 +951,8 @@
         <v>1.5210906168970626</v>
       </c>
       <c r="M4" s="14">
-        <f t="shared" ref="M4:M11" si="0">J4/(D4*1000)</f>
-        <v>1.9006030299093645E-5</v>
+        <f t="shared" ref="M4:M11" si="0">(1000*J4)/D4</f>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -984,7 +990,7 @@
       </c>
       <c r="M5" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1024,12 +1030,12 @@
         <v>1.8340522384700824</v>
       </c>
       <c r="L6" s="14">
-        <f t="shared" ref="L5:L11" si="3">I6/(1000*E6)</f>
-        <v>9.7397515923315907E-4</v>
+        <f>(I6*1000)/E6</f>
+        <v>973.97515923315905</v>
       </c>
       <c r="M6" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1056,7 +1062,7 @@
         <v>80.86</v>
       </c>
       <c r="H7" s="27">
-        <f t="shared" ref="H7:H8" si="4">160-G8</f>
+        <f t="shared" ref="H7:H8" si="3">160-G8</f>
         <v>79.023600000000002</v>
       </c>
       <c r="I7" s="20">
@@ -1069,12 +1075,12 @@
         <v>1.8345015054549394</v>
       </c>
       <c r="L7" s="14">
-        <f t="shared" si="3"/>
-        <v>9.7397515923315896E-4</v>
+        <f t="shared" ref="L7:L11" si="4">(I7*1000)/E7</f>
+        <v>973.97515923315916</v>
       </c>
       <c r="M7" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1101,7 +1107,7 @@
         <v>80.976399999999998</v>
       </c>
       <c r="H8" s="27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>79.011600000000001</v>
       </c>
       <c r="I8" s="29">
@@ -1114,12 +1120,12 @@
         <v>1.8324720373115726</v>
       </c>
       <c r="L8" s="14">
-        <f t="shared" si="3"/>
-        <v>9.7397515923315907E-4</v>
+        <f t="shared" si="4"/>
+        <v>973.97515923315905</v>
       </c>
       <c r="M8" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1147,7 +1153,7 @@
       </c>
       <c r="H9" s="27">
         <f>160-G11</f>
-        <v>160</v>
+        <v>79.011600000000001</v>
       </c>
       <c r="I9" s="29">
         <v>0.78894051804324872</v>
@@ -1159,12 +1165,12 @@
         <v>1.9273905007195093</v>
       </c>
       <c r="L9" s="14">
-        <f t="shared" si="3"/>
-        <v>8.130054802589125E-4</v>
+        <f t="shared" si="4"/>
+        <v>813.00548025891248</v>
       </c>
       <c r="M9" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1187,8 +1193,8 @@
         <v>0</v>
       </c>
       <c r="G10" s="27">
-        <f t="shared" si="5"/>
-        <v>0</v>
+        <f>SUM(D10:F10)</f>
+        <v>81.017800000000008</v>
       </c>
       <c r="H10" s="27">
         <f t="shared" ref="H10:H11" si="6">160-G12</f>
@@ -1204,12 +1210,12 @@
         <v>1.9295953770092844</v>
       </c>
       <c r="L10" s="14">
-        <f t="shared" si="3"/>
-        <v>8.1300548025891261E-4</v>
+        <f t="shared" si="4"/>
+        <v>813.00548025891248</v>
       </c>
       <c r="M10" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1232,8 +1238,8 @@
         <v>0</v>
       </c>
       <c r="G11" s="27">
-        <f>SUM(D13:F13)</f>
-        <v>0</v>
+        <f>SUM(D11:F11)</f>
+        <v>80.988399999999999</v>
       </c>
       <c r="H11" s="27">
         <f t="shared" si="6"/>
@@ -1249,12 +1255,12 @@
         <v>1.9296922316001799</v>
       </c>
       <c r="L11" s="14">
-        <f t="shared" si="3"/>
-        <v>8.1300548025891239E-4</v>
+        <f t="shared" si="4"/>
+        <v>813.00548025891248</v>
       </c>
       <c r="M11" s="14">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -5337,8 +5343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5455,22 +5461,36 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
     </row>
-    <row r="20" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C22" s="10"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D23" s="13"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D25" s="13"/>
     </row>
   </sheetData>

</xml_diff>